<commit_message>
agni, jsl, gazi cdr processed
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sftp_root\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="NE automation data" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -985,7 +985,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13">
     <font>
       <sz val="10"/>
@@ -1415,12 +1415,12 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickTop="1" thickBot="1">
+    <row r="1" spans="1:22" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" thickTop="1">
+    <row r="2" spans="1:22" ht="15.75" thickTop="1">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -1520,8 +1520,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="19">
-        <f t="array" ref="K2">INDEX(Sheet2!$H$2:$I$21,MATCH(G2,Sheet2!$I$2:I6,0),1)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="20" t="str">
         <f t="array" ref="L2">INDEX(Sheet2!$B$2:$C$21,MATCH(G2,Sheet2!$C$2:C21,0),1)</f>
@@ -1559,7 +1558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.4">
+    <row r="3" spans="1:22" ht="15">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="14.4">
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
@@ -1701,7 +1700,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="14.4">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="15" t="s">
         <v>37</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14.4">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="15" t="s">
         <v>50</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.4">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="15" t="s">
         <v>50</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.4">
+    <row r="8" spans="1:22" ht="15">
       <c r="A8" s="15" t="s">
         <v>62</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.4">
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="15" t="s">
         <v>62</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.4">
+    <row r="10" spans="1:22" ht="15">
       <c r="A10" s="15" t="s">
         <v>72</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.4">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="15" t="s">
         <v>72</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="14.4">
+    <row r="12" spans="1:22" ht="15">
       <c r="A12" s="15" t="s">
         <v>72</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="14.4">
+    <row r="13" spans="1:22" ht="15">
       <c r="A13" s="15" t="s">
         <v>88</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="14.4">
+    <row r="14" spans="1:22" ht="15">
       <c r="A14" s="15" t="s">
         <v>88</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="14.4">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="15" t="s">
         <v>99</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.4">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="15" t="s">
         <v>99</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="14.4">
+    <row r="17" spans="1:22" ht="15">
       <c r="A17" s="15" t="s">
         <v>111</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="14.4">
+    <row r="18" spans="1:22" ht="15">
       <c r="A18" s="15" t="s">
         <v>111</v>
       </c>
@@ -2695,7 +2694,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="14.4">
+    <row r="19" spans="1:22" ht="15">
       <c r="A19" s="15" t="s">
         <v>122</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="14.4">
+    <row r="20" spans="1:22" ht="15">
       <c r="A20" s="15" t="s">
         <v>122</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="14.4">
+    <row r="21" spans="1:22" ht="15">
       <c r="A21" s="15" t="s">
         <v>132</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="14.4">
+    <row r="22" spans="1:22" ht="15">
       <c r="A22" s="15" t="s">
         <v>132</v>
       </c>
@@ -2979,7 +2978,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="14.4">
+    <row r="23" spans="1:22" ht="15">
       <c r="A23" s="15" t="s">
         <v>143</v>
       </c>
@@ -3048,7 +3047,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="14.4">
+    <row r="24" spans="1:22" ht="15">
       <c r="A24" s="15" t="s">
         <v>143</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="14.4">
+    <row r="25" spans="1:22" ht="15">
       <c r="A25" s="15" t="s">
         <v>154</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="14.4">
+    <row r="26" spans="1:22" ht="15">
       <c r="A26" s="15" t="s">
         <v>154</v>
       </c>
@@ -3261,7 +3260,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="14.4">
+    <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
         <v>165</v>
       </c>
@@ -3332,7 +3331,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="14.4">
+    <row r="28" spans="1:22" ht="15">
       <c r="A28" s="15" t="s">
         <v>165</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="14.4">
+    <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
         <v>175</v>
       </c>
@@ -3474,7 +3473,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="14.4">
+    <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
         <v>175</v>
       </c>
@@ -3545,7 +3544,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="14.4">
+    <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
         <v>187</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="14.4">
+    <row r="32" spans="1:22" ht="15">
       <c r="A32" s="15" t="s">
         <v>187</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="14.4">
+    <row r="33" spans="1:22" ht="15">
       <c r="A33" s="15" t="s">
         <v>187</v>
       </c>
@@ -3758,7 +3757,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="14.4">
+    <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
         <v>203</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="14.4">
+    <row r="35" spans="1:22" ht="15">
       <c r="A35" s="15" t="s">
         <v>203</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="14.4">
+    <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
         <v>212</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="14.4">
+    <row r="37" spans="1:22" ht="15">
       <c r="A37" s="15" t="s">
         <v>212</v>
       </c>
@@ -4042,7 +4041,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="14.4">
+    <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
         <v>223</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="14.4">
+    <row r="39" spans="1:22" ht="15">
       <c r="A39" s="15" t="s">
         <v>223</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="14.4">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
         <v>234</v>
       </c>
@@ -4255,7 +4254,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="14.4">
+    <row r="41" spans="1:22" ht="15">
       <c r="A41" s="15" t="s">
         <v>234</v>
       </c>
@@ -4326,7 +4325,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="14.4">
+    <row r="42" spans="1:22" ht="15">
       <c r="A42" s="15" t="s">
         <v>234</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="14.4">
+    <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
         <v>250</v>
       </c>
@@ -4468,7 +4467,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="14.4">
+    <row r="44" spans="1:22" ht="15">
       <c r="A44" s="15" t="s">
         <v>250</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="14.4">
+    <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
         <v>261</v>
       </c>
@@ -4610,7 +4609,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="14.4">
+    <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
         <v>261</v>
       </c>
@@ -4681,7 +4680,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="14.4">
+    <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
         <v>271</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="14.4">
+    <row r="48" spans="1:22" ht="15">
       <c r="A48" s="15" t="s">
         <v>271</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="14.4">
+    <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
         <v>283</v>
       </c>
@@ -4893,7 +4892,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="14.4">
+    <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
         <v>283</v>
       </c>
@@ -4964,7 +4963,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="14.4">
+    <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
         <v>292</v>
       </c>
@@ -5035,7 +5034,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="14.4">
+    <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
         <v>292</v>
       </c>
@@ -5119,11 +5118,11 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Add .conf in git ignore
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -1445,9 +1445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1804,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="T5" s="16">
         <v>0</v>

</xml_diff>

<commit_message>
Domestic data in loop
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sftp_root\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAS\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F731B75-6D2E-422F-A85D-896E1F39A4F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NE automation data" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -988,7 +989,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13">
     <font>
       <sz val="10"/>
@@ -1442,12 +1443,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3847,10 +3848,10 @@
         <v>27</v>
       </c>
       <c r="O34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="16">
         <v>1</v>
@@ -3865,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="U34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34" s="15" t="s">
         <v>203</v>
@@ -3917,10 +3918,10 @@
         <v>35</v>
       </c>
       <c r="O35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q35" s="16">
         <v>1</v>
@@ -3935,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="U35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V35" s="15" t="s">
         <v>203</v>
@@ -5153,7 +5154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
paradise and sheba configured
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sftproot\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="322">
   <si>
     <t>operator</t>
   </si>
@@ -505,9 +505,6 @@
     <t>g:\telcobright\vault\resources\cdr\paradise\tdm</t>
   </si>
   <si>
-    <t>paradise_10.154.150.36_HUWAEI</t>
-  </si>
-  <si>
     <t>purple</t>
   </si>
   <si>
@@ -670,9 +667,6 @@
     <t>i:\telcobright\vault\resources\cdr\sheba\tdm</t>
   </si>
   <si>
-    <t>sheba_10.154.150.51_HUWAEI</t>
-  </si>
-  <si>
     <t>softex</t>
   </si>
   <si>
@@ -989,6 +983,9 @@
   </si>
   <si>
     <t>e:\telcobright\vault\resources\cdr\telePlusNewyork\tdm</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -1454,9 +1451,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1675,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1817,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="T5" s="16">
         <v>0</v>
@@ -2100,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T9" s="16">
         <v>0</v>
@@ -2573,7 +2570,7 @@
         <v>17</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M16" s="21" t="str">
         <f t="array" ref="M16">INDEX(Sheet2!$E$2:$F$21,MATCH(G16,Sheet2!$F$2:F35,0),1)</f>
@@ -2996,7 +2993,7 @@
         <v>51</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M22" s="21" t="str">
         <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F41,0),1)</f>
@@ -3018,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T22" s="16">
         <v>0</v>
@@ -3276,9 +3273,8 @@
         <f t="array" ref="K26">INDEX(Sheet2!$H$2:$I$21,MATCH(G26,Sheet2!$I$2:I30,0),1)</f>
         <v>3</v>
       </c>
-      <c r="L26" s="20" t="str">
-        <f t="array" ref="L26">INDEX(Sheet2!$B$2:$C$21,MATCH(G26,Sheet2!$C$2:C45,0),1)</f>
-        <v>b</v>
+      <c r="L26" s="20" t="s">
+        <v>321</v>
       </c>
       <c r="M26" s="21" t="str">
         <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F45,0),1)</f>
@@ -3288,10 +3284,10 @@
         <v>27</v>
       </c>
       <c r="O26" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="16">
         <v>1</v>
@@ -3300,13 +3296,13 @@
         <v>1</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>161</v>
+        <v>310</v>
       </c>
       <c r="T26" s="16">
         <v>0</v>
       </c>
       <c r="U26" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="15" t="s">
         <v>151</v>
@@ -3314,7 +3310,7 @@
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B27" s="16">
         <v>16</v>
@@ -3326,19 +3322,19 @@
         <v>4</v>
       </c>
       <c r="E27" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="J27" s="16">
         <v>16</v>
@@ -3380,12 +3376,12 @@
         <v>1</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15">
       <c r="A28" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B28" s="16">
         <v>16</v>
@@ -3397,19 +3393,19 @@
         <v>29</v>
       </c>
       <c r="E28" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H28" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="I28" s="15" t="s">
         <v>169</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>170</v>
       </c>
       <c r="J28" s="16">
         <v>16</v>
@@ -3419,7 +3415,7 @@
         <v>3</v>
       </c>
       <c r="L28" s="20" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M28" s="21" t="str">
         <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F47,0),1)</f>
@@ -3441,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="T28" s="16">
         <v>0</v>
@@ -3450,12 +3446,12 @@
         <v>0</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="16">
         <v>17</v>
@@ -3467,19 +3463,19 @@
         <v>4</v>
       </c>
       <c r="E29" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="G29" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="H29" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>175</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>176</v>
       </c>
       <c r="J29" s="16">
         <v>17</v>
@@ -3512,7 +3508,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3521,12 +3517,12 @@
         <v>1</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B30" s="16">
         <v>17</v>
@@ -3538,19 +3534,19 @@
         <v>29</v>
       </c>
       <c r="E30" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>178</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>179</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>106</v>
       </c>
       <c r="H30" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="I30" s="15" t="s">
         <v>180</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>181</v>
       </c>
       <c r="J30" s="16">
         <v>17</v>
@@ -3560,7 +3556,7 @@
         <v>17</v>
       </c>
       <c r="L30" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M30" s="21" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G30,Sheet2!$F$2:F49,0),1)</f>
@@ -3582,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="T30" s="16">
         <v>0</v>
@@ -3591,12 +3587,12 @@
         <v>0</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" s="16">
         <v>18</v>
@@ -3608,19 +3604,19 @@
         <v>4</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>184</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H31" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>186</v>
       </c>
       <c r="J31" s="16">
         <v>18</v>
@@ -3661,12 +3657,12 @@
         <v>0</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
       <c r="A32" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B32" s="16">
         <v>18</v>
@@ -3678,19 +3674,19 @@
         <v>29</v>
       </c>
       <c r="E32" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>32</v>
       </c>
       <c r="H32" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="I32" s="15" t="s">
         <v>189</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>190</v>
       </c>
       <c r="J32" s="16">
         <v>18</v>
@@ -3723,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T32" s="16">
         <v>0</v>
@@ -3732,12 +3728,12 @@
         <v>1</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15">
       <c r="A33" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" s="16">
         <v>18</v>
@@ -3749,19 +3745,19 @@
         <v>29</v>
       </c>
       <c r="E33" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>192</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>193</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>84</v>
       </c>
       <c r="H33" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>194</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>195</v>
       </c>
       <c r="J33" s="16">
         <v>18</v>
@@ -3794,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
@@ -3803,12 +3799,12 @@
         <v>1</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B34" s="16">
         <v>19</v>
@@ -3820,19 +3816,19 @@
         <v>4</v>
       </c>
       <c r="E34" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>199</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H34" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="J34" s="16">
         <v>19</v>
@@ -3874,12 +3870,12 @@
         <v>1</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
       <c r="A35" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="16">
         <v>19</v>
@@ -3891,19 +3887,19 @@
         <v>29</v>
       </c>
       <c r="E35" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>202</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>203</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H35" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>204</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="J35" s="16">
         <v>19</v>
@@ -3913,7 +3909,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M35" s="21" t="str">
         <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F54,0),1)</f>
@@ -3944,12 +3940,12 @@
         <v>0</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B36" s="16">
         <v>20</v>
@@ -3961,19 +3957,19 @@
         <v>4</v>
       </c>
       <c r="E36" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>208</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H36" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I36" s="15" t="s">
         <v>209</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>210</v>
       </c>
       <c r="J36" s="16">
         <v>20</v>
@@ -4006,7 +4002,7 @@
         <v>1</v>
       </c>
       <c r="S36" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T36" s="16">
         <v>0</v>
@@ -4015,12 +4011,12 @@
         <v>1</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15">
       <c r="A37" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B37" s="16">
         <v>20</v>
@@ -4032,19 +4028,19 @@
         <v>29</v>
       </c>
       <c r="E37" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="15" t="s">
         <v>212</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>213</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H37" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="I37" s="15" t="s">
         <v>214</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>215</v>
       </c>
       <c r="J37" s="16">
         <v>20</v>
@@ -4053,9 +4049,8 @@
         <f t="array" ref="K37">INDEX(Sheet2!$H$2:$I$21,MATCH(G37,Sheet2!$I$2:I41,0),1)</f>
         <v>3</v>
       </c>
-      <c r="L37" s="20" t="str">
-        <f t="array" ref="L37">INDEX(Sheet2!$B$2:$C$21,MATCH(G37,Sheet2!$C$2:C56,0),1)</f>
-        <v>b</v>
+      <c r="L37" s="20" t="s">
+        <v>297</v>
       </c>
       <c r="M37" s="21" t="str">
         <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F56,0),1)</f>
@@ -4065,10 +4060,10 @@
         <v>27</v>
       </c>
       <c r="O37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="16">
         <v>1</v>
@@ -4077,21 +4072,21 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>216</v>
+        <v>310</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
       </c>
       <c r="U37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V37" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B38" s="16">
         <v>21</v>
@@ -4103,19 +4098,19 @@
         <v>4</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J38" s="16">
         <v>21</v>
@@ -4148,7 +4143,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4157,12 +4152,12 @@
         <v>0</v>
       </c>
       <c r="V38" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
       <c r="A39" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B39" s="16">
         <v>21</v>
@@ -4174,19 +4169,19 @@
         <v>29</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J39" s="16">
         <v>21</v>
@@ -4219,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
@@ -4228,12 +4223,12 @@
         <v>0</v>
       </c>
       <c r="V39" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="16">
         <v>22</v>
@@ -4245,19 +4240,19 @@
         <v>4</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J40" s="16">
         <v>22</v>
@@ -4290,7 +4285,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="T40" s="16">
         <v>0</v>
@@ -4299,12 +4294,12 @@
         <v>1</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15">
       <c r="A41" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B41" s="16">
         <v>22</v>
@@ -4316,19 +4311,19 @@
         <v>29</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J41" s="16">
         <v>22</v>
@@ -4361,7 +4356,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
@@ -4370,12 +4365,12 @@
         <v>1</v>
       </c>
       <c r="V41" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15">
       <c r="A42" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B42" s="16">
         <v>22</v>
@@ -4387,19 +4382,19 @@
         <v>29</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>84</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J42" s="16">
         <v>22</v>
@@ -4432,7 +4427,7 @@
         <v>1</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
@@ -4441,12 +4436,12 @@
         <v>1</v>
       </c>
       <c r="V42" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B43" s="16">
         <v>23</v>
@@ -4458,19 +4453,19 @@
         <v>4</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J43" s="16">
         <v>23</v>
@@ -4512,12 +4507,12 @@
         <v>1</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15">
       <c r="A44" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B44" s="16">
         <v>23</v>
@@ -4529,19 +4524,19 @@
         <v>29</v>
       </c>
       <c r="E44" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="G44" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="H44" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="I44" s="15" t="s">
         <v>250</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>252</v>
       </c>
       <c r="J44" s="16">
         <v>23</v>
@@ -4574,7 +4569,7 @@
         <v>1</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="T44" s="16">
         <v>0</v>
@@ -4583,12 +4578,12 @@
         <v>1</v>
       </c>
       <c r="V44" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B45" s="16">
         <v>24</v>
@@ -4600,19 +4595,19 @@
         <v>4</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J45" s="16">
         <v>24</v>
@@ -4645,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T45" s="16">
         <v>1</v>
@@ -4654,12 +4649,12 @@
         <v>1</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B46" s="16">
         <v>24</v>
@@ -4671,19 +4666,19 @@
         <v>29</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="H46" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="I46" s="15" t="s">
         <v>261</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>263</v>
       </c>
       <c r="J46" s="16">
         <v>24</v>
@@ -4725,12 +4720,12 @@
         <v>1</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B47" s="16">
         <v>25</v>
@@ -4742,19 +4737,19 @@
         <v>4</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="H47" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="I47" s="15" t="s">
         <v>319</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>321</v>
       </c>
       <c r="J47" s="16">
         <v>25</v>
@@ -4768,7 +4763,7 @@
         <v>2</v>
       </c>
       <c r="M47" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N47" s="15" t="s">
         <v>27</v>
@@ -4795,12 +4790,12 @@
         <v>1</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15">
       <c r="A48" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B48" s="16">
         <v>25</v>
@@ -4812,19 +4807,19 @@
         <v>29</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J48" s="16">
         <v>25</v>
@@ -4856,7 +4851,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="T48" s="16">
         <v>0</v>
@@ -4865,12 +4860,12 @@
         <v>0</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B49" s="16">
         <v>26</v>
@@ -4882,19 +4877,19 @@
         <v>4</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J49" s="16">
         <v>26</v>
@@ -4936,12 +4931,12 @@
         <v>1</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B50" s="16">
         <v>26</v>
@@ -4953,19 +4948,19 @@
         <v>29</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>106</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J50" s="16">
         <v>26</v>
@@ -4998,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="T50" s="16">
         <v>0</v>
@@ -5007,12 +5002,12 @@
         <v>0</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B51" s="16">
         <v>27</v>
@@ -5024,19 +5019,19 @@
         <v>4</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J51" s="16">
         <v>27</v>
@@ -5078,12 +5073,12 @@
         <v>1</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B52" s="16">
         <v>27</v>
@@ -5095,19 +5090,19 @@
         <v>29</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J52" s="16">
         <v>27</v>
@@ -5139,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="S52" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="T52" s="16">
         <v>0</v>
@@ -5148,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5175,24 +5170,24 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5214,14 +5209,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5236,14 +5231,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5258,14 +5253,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -5280,14 +5275,14 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>106</v>
@@ -5302,14 +5297,14 @@
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5324,36 +5319,36 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8">
         <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5368,14 +5363,14 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>84</v>
@@ -5393,41 +5388,41 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
         <v>39</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
@@ -5535,7 +5530,7 @@
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
       <c r="C25" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>

</xml_diff>

<commit_message>
gazi genband decoder added
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="325">
   <si>
     <t>operator</t>
   </si>
@@ -265,9 +265,6 @@
     <t>d:\telcobright\vault\resources\cdr\gaziNetworks\tdm</t>
   </si>
   <si>
-    <t>Vault.GenbandDhk</t>
-  </si>
-  <si>
     <t>10.154.150.9</t>
   </si>
   <si>
@@ -995,6 +992,9 @@
   </si>
   <si>
     <t>.cdr</t>
+  </si>
+  <si>
+    <t>GAZI</t>
   </si>
 </sst>
 </file>
@@ -1460,9 +1460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
+      <selection pane="bottomLeft" activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1681,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T5" s="16">
         <v>0</v>
@@ -1941,7 +1941,7 @@
         <v>49</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="15" t="s">
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T9" s="16">
         <v>0</v>
@@ -2215,25 +2215,20 @@
         <v>6</v>
       </c>
       <c r="K11" s="19">
-        <f t="array" ref="K11">INDEX(Sheet2!$H$2:$I$21,MATCH(G11,Sheet2!$I$2:I15,0),1)</f>
-        <v>31</v>
-      </c>
-      <c r="L11" s="20" t="str">
-        <f t="array" ref="L11">INDEX(Sheet2!$B$2:$C$21,MATCH(G11,Sheet2!$C$2:C30,0),1)</f>
-        <v>VCDR</v>
-      </c>
-      <c r="M11" s="21" t="str">
-        <f t="array" ref="M11">INDEX(Sheet2!$E$2:$F$21,MATCH(G11,Sheet2!$F$2:F30,0),1)</f>
-        <v>.gz</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="M11" s="21"/>
       <c r="N11" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O11" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="16">
         <v>1</v>
@@ -2242,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="T11" s="16">
         <v>0</v>
@@ -2268,19 +2263,19 @@
         <v>29</v>
       </c>
       <c r="E12" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="G12" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="H12" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>86</v>
       </c>
       <c r="J12" s="16">
         <v>6</v>
@@ -2313,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T12" s="16">
         <v>0</v>
@@ -2327,7 +2322,7 @@
     </row>
     <row r="13" spans="1:22" ht="15">
       <c r="A13" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="16">
         <v>7</v>
@@ -2339,19 +2334,19 @@
         <v>4</v>
       </c>
       <c r="E13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>91</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>92</v>
       </c>
       <c r="J13" s="16">
         <v>7</v>
@@ -2384,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T13" s="16">
         <v>0</v>
@@ -2393,12 +2388,12 @@
         <v>0</v>
       </c>
       <c r="V13" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15">
       <c r="A14" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="16">
         <v>7</v>
@@ -2410,19 +2405,19 @@
         <v>29</v>
       </c>
       <c r="E14" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>97</v>
       </c>
       <c r="J14" s="16">
         <v>7</v>
@@ -2455,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T14" s="16">
         <v>0</v>
@@ -2464,12 +2459,12 @@
         <v>0</v>
       </c>
       <c r="V14" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15">
       <c r="A15" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="16">
         <v>8</v>
@@ -2481,19 +2476,19 @@
         <v>4</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H15" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="J15" s="16">
         <v>8</v>
@@ -2526,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T15" s="16">
         <v>0</v>
@@ -2535,12 +2530,12 @@
         <v>1</v>
       </c>
       <c r="V15" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
       <c r="A16" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="16">
         <v>8</v>
@@ -2552,19 +2547,19 @@
         <v>29</v>
       </c>
       <c r="E16" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="G16" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="I16" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="J16" s="16">
         <v>8</v>
@@ -2574,7 +2569,7 @@
         <v>17</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M16" s="21" t="str">
         <f t="array" ref="M16">INDEX(Sheet2!$E$2:$F$21,MATCH(G16,Sheet2!$F$2:F35,0),1)</f>
@@ -2596,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T16" s="16">
         <v>0</v>
@@ -2605,12 +2600,12 @@
         <v>0</v>
       </c>
       <c r="V16" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
       <c r="A17" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="16">
         <v>9</v>
@@ -2622,19 +2617,19 @@
         <v>4</v>
       </c>
       <c r="E17" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H17" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="J17" s="16">
         <v>9</v>
@@ -2666,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T17" s="16">
         <v>0</v>
@@ -2675,12 +2670,12 @@
         <v>0</v>
       </c>
       <c r="V17" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
       <c r="A18" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="16">
         <v>9</v>
@@ -2692,19 +2687,19 @@
         <v>29</v>
       </c>
       <c r="E18" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="G18" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>118</v>
       </c>
       <c r="J18" s="16">
         <v>9</v>
@@ -2737,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T18" s="16">
         <v>0</v>
@@ -2746,12 +2741,12 @@
         <v>0</v>
       </c>
       <c r="V18" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15">
       <c r="A19" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="16">
         <v>10</v>
@@ -2763,19 +2758,19 @@
         <v>4</v>
       </c>
       <c r="E19" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H19" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>124</v>
       </c>
       <c r="J19" s="16">
         <v>10</v>
@@ -2808,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T19" s="16">
         <v>0</v>
@@ -2817,12 +2812,12 @@
         <v>1</v>
       </c>
       <c r="V19" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15">
       <c r="A20" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="16">
         <v>10</v>
@@ -2834,19 +2829,19 @@
         <v>29</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F20" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J20" s="16">
         <v>10</v>
@@ -2879,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T20" s="16">
         <v>0</v>
@@ -2888,12 +2883,12 @@
         <v>1</v>
       </c>
       <c r="V20" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15">
       <c r="A21" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="16">
         <v>11</v>
@@ -2905,19 +2900,19 @@
         <v>4</v>
       </c>
       <c r="E21" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>131</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>132</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H21" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>134</v>
       </c>
       <c r="J21" s="16">
         <v>11</v>
@@ -2950,7 +2945,7 @@
         <v>1</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T21" s="16">
         <v>0</v>
@@ -2959,12 +2954,12 @@
         <v>1</v>
       </c>
       <c r="V21" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15">
       <c r="A22" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22" s="16">
         <v>11</v>
@@ -2976,19 +2971,19 @@
         <v>29</v>
       </c>
       <c r="E22" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H22" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="J22" s="16">
         <v>11</v>
@@ -2997,7 +2992,7 @@
         <v>51</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M22" s="21" t="str">
         <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F41,0),1)</f>
@@ -3019,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T22" s="16">
         <v>0</v>
@@ -3028,12 +3023,12 @@
         <v>0</v>
       </c>
       <c r="V22" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="32" customFormat="1" ht="15">
       <c r="A23" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B23" s="27">
         <v>12</v>
@@ -3045,17 +3040,17 @@
         <v>4</v>
       </c>
       <c r="E23" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="26" t="s">
         <v>141</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>142</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>143</v>
-      </c>
-      <c r="I23" s="26" t="s">
-        <v>144</v>
       </c>
       <c r="J23" s="27">
         <v>12</v>
@@ -3088,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="S23" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T23" s="27">
         <v>0</v>
@@ -3097,12 +3092,12 @@
         <v>1</v>
       </c>
       <c r="V23" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15">
       <c r="A24" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" s="16">
         <v>12</v>
@@ -3114,19 +3109,19 @@
         <v>29</v>
       </c>
       <c r="E24" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H24" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" s="15" t="s">
         <v>148</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>149</v>
       </c>
       <c r="J24" s="16">
         <v>12</v>
@@ -3159,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T24" s="16">
         <v>0</v>
@@ -3168,12 +3163,12 @@
         <v>1</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15">
       <c r="A25" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B25" s="16">
         <v>15</v>
@@ -3185,19 +3180,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H25" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>154</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>155</v>
       </c>
       <c r="J25" s="16">
         <v>15</v>
@@ -3230,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T25" s="16">
         <v>0</v>
@@ -3239,12 +3234,12 @@
         <v>1</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15">
       <c r="A26" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26" s="16">
         <v>15</v>
@@ -3256,19 +3251,19 @@
         <v>29</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H26" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="J26" s="16">
         <v>15</v>
@@ -3278,7 +3273,7 @@
         <v>3</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M26" s="21" t="str">
         <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F45,0),1)</f>
@@ -3300,7 +3295,7 @@
         <v>1</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T26" s="16">
         <v>0</v>
@@ -3309,12 +3304,12 @@
         <v>0</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B27" s="16">
         <v>16</v>
@@ -3326,19 +3321,19 @@
         <v>4</v>
       </c>
       <c r="E27" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="J27" s="16">
         <v>16</v>
@@ -3380,12 +3375,12 @@
         <v>1</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15">
       <c r="A28" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" s="16">
         <v>16</v>
@@ -3397,19 +3392,19 @@
         <v>29</v>
       </c>
       <c r="E28" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>167</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H28" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="J28" s="16">
         <v>16</v>
@@ -3419,7 +3414,7 @@
         <v>3</v>
       </c>
       <c r="L28" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M28" s="21" t="str">
         <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F47,0),1)</f>
@@ -3441,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T28" s="16">
         <v>0</v>
@@ -3450,12 +3445,12 @@
         <v>0</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="16">
         <v>17</v>
@@ -3467,19 +3462,19 @@
         <v>4</v>
       </c>
       <c r="E29" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="G29" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="H29" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>174</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>175</v>
       </c>
       <c r="J29" s="16">
         <v>17</v>
@@ -3491,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N29" s="15" t="s">
         <v>27</v>
@@ -3509,7 +3504,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3518,12 +3513,12 @@
         <v>0</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="16">
         <v>17</v>
@@ -3535,19 +3530,19 @@
         <v>29</v>
       </c>
       <c r="E30" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="G30" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>178</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>179</v>
       </c>
       <c r="J30" s="16">
         <v>17</v>
@@ -3557,7 +3552,7 @@
         <v>17</v>
       </c>
       <c r="L30" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M30" s="21" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G30,Sheet2!$F$2:F49,0),1)</f>
@@ -3579,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="T30" s="16">
         <v>0</v>
@@ -3588,12 +3583,12 @@
         <v>0</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B31" s="16">
         <v>18</v>
@@ -3605,19 +3600,19 @@
         <v>4</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>182</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H31" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>184</v>
       </c>
       <c r="J31" s="16">
         <v>18</v>
@@ -3658,12 +3653,12 @@
         <v>0</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
       <c r="A32" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="16">
         <v>18</v>
@@ -3675,19 +3670,19 @@
         <v>29</v>
       </c>
       <c r="E32" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>186</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>32</v>
       </c>
       <c r="H32" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I32" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="J32" s="16">
         <v>18</v>
@@ -3720,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T32" s="16">
         <v>0</v>
@@ -3729,12 +3724,12 @@
         <v>1</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15">
       <c r="A33" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B33" s="16">
         <v>18</v>
@@ -3746,19 +3741,19 @@
         <v>29</v>
       </c>
       <c r="E33" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="G33" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="15" t="s">
+      <c r="I33" s="15" t="s">
         <v>192</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>193</v>
       </c>
       <c r="J33" s="16">
         <v>18</v>
@@ -3791,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
@@ -3800,12 +3795,12 @@
         <v>1</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B34" s="16">
         <v>19</v>
@@ -3817,19 +3812,19 @@
         <v>4</v>
       </c>
       <c r="E34" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>196</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>197</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H34" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>199</v>
       </c>
       <c r="J34" s="16">
         <v>19</v>
@@ -3871,12 +3866,12 @@
         <v>1</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
       <c r="A35" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" s="16">
         <v>19</v>
@@ -3888,19 +3883,19 @@
         <v>29</v>
       </c>
       <c r="E35" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H35" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>202</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>203</v>
       </c>
       <c r="J35" s="16">
         <v>19</v>
@@ -3910,7 +3905,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M35" s="21" t="str">
         <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F54,0),1)</f>
@@ -3941,12 +3936,12 @@
         <v>0</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B36" s="16">
         <v>20</v>
@@ -3958,19 +3953,19 @@
         <v>4</v>
       </c>
       <c r="E36" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F36" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>206</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H36" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="I36" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>208</v>
       </c>
       <c r="J36" s="16">
         <v>20</v>
@@ -4003,7 +3998,7 @@
         <v>1</v>
       </c>
       <c r="S36" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T36" s="16">
         <v>0</v>
@@ -4012,12 +4007,12 @@
         <v>1</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15">
       <c r="A37" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" s="16">
         <v>20</v>
@@ -4029,19 +4024,19 @@
         <v>29</v>
       </c>
       <c r="E37" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37" s="15" t="s">
         <v>210</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>211</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H37" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="I37" s="15" t="s">
         <v>212</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>213</v>
       </c>
       <c r="J37" s="16">
         <v>20</v>
@@ -4051,7 +4046,7 @@
         <v>3</v>
       </c>
       <c r="L37" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M37" s="21" t="str">
         <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F56,0),1)</f>
@@ -4073,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
@@ -4082,12 +4077,12 @@
         <v>0</v>
       </c>
       <c r="V37" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" s="16">
         <v>21</v>
@@ -4099,19 +4094,19 @@
         <v>4</v>
       </c>
       <c r="E38" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" s="15" t="s">
         <v>215</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>216</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H38" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="I38" s="15" t="s">
         <v>217</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>218</v>
       </c>
       <c r="J38" s="16">
         <v>21</v>
@@ -4144,7 +4139,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4153,12 +4148,12 @@
         <v>0</v>
       </c>
       <c r="V38" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
       <c r="A39" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39" s="16">
         <v>21</v>
@@ -4170,19 +4165,19 @@
         <v>29</v>
       </c>
       <c r="E39" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>221</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H39" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="I39" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>223</v>
       </c>
       <c r="J39" s="16">
         <v>21</v>
@@ -4215,7 +4210,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
@@ -4224,12 +4219,12 @@
         <v>0</v>
       </c>
       <c r="V39" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B40" s="16">
         <v>22</v>
@@ -4241,19 +4236,19 @@
         <v>4</v>
       </c>
       <c r="E40" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F40" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>226</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H40" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="I40" s="15" t="s">
         <v>227</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>228</v>
       </c>
       <c r="J40" s="16">
         <v>22</v>
@@ -4286,7 +4281,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T40" s="16">
         <v>0</v>
@@ -4295,12 +4290,12 @@
         <v>1</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15">
       <c r="A41" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B41" s="16">
         <v>22</v>
@@ -4312,19 +4307,19 @@
         <v>29</v>
       </c>
       <c r="E41" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F41" s="15" t="s">
         <v>230</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>231</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H41" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="I41" s="15" t="s">
         <v>232</v>
-      </c>
-      <c r="I41" s="15" t="s">
-        <v>233</v>
       </c>
       <c r="J41" s="16">
         <v>22</v>
@@ -4357,7 +4352,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
@@ -4366,12 +4361,12 @@
         <v>1</v>
       </c>
       <c r="V41" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15">
       <c r="A42" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" s="16">
         <v>22</v>
@@ -4383,19 +4378,19 @@
         <v>29</v>
       </c>
       <c r="E42" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="F42" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="G42" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="G42" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42" s="15" t="s">
+      <c r="I42" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="I42" s="15" t="s">
-        <v>238</v>
       </c>
       <c r="J42" s="16">
         <v>22</v>
@@ -4428,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
@@ -4437,12 +4432,12 @@
         <v>1</v>
       </c>
       <c r="V42" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B43" s="16">
         <v>23</v>
@@ -4454,19 +4449,19 @@
         <v>4</v>
       </c>
       <c r="E43" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F43" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H43" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="I43" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>244</v>
       </c>
       <c r="J43" s="16">
         <v>23</v>
@@ -4499,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T43" s="16">
         <v>0</v>
@@ -4508,12 +4503,12 @@
         <v>1</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15">
       <c r="A44" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B44" s="16">
         <v>23</v>
@@ -4525,19 +4520,19 @@
         <v>29</v>
       </c>
       <c r="E44" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F44" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="G44" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="H44" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="H44" s="15" t="s">
+      <c r="I44" s="15" t="s">
         <v>248</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>249</v>
       </c>
       <c r="J44" s="16">
         <v>23</v>
@@ -4570,7 +4565,7 @@
         <v>1</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T44" s="16">
         <v>0</v>
@@ -4579,12 +4574,12 @@
         <v>1</v>
       </c>
       <c r="V44" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B45" s="16">
         <v>24</v>
@@ -4596,19 +4591,19 @@
         <v>4</v>
       </c>
       <c r="E45" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F45" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="F45" s="15" t="s">
-        <v>253</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H45" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="I45" s="15" t="s">
         <v>254</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>255</v>
       </c>
       <c r="J45" s="16">
         <v>24</v>
@@ -4641,7 +4636,7 @@
         <v>1</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T45" s="16">
         <v>1</v>
@@ -4650,12 +4645,12 @@
         <v>1</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B46" s="16">
         <v>24</v>
@@ -4667,19 +4662,19 @@
         <v>29</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F46" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="G46" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="G46" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="H46" s="15" t="s">
+      <c r="I46" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="J46" s="16">
         <v>24</v>
@@ -4721,12 +4716,12 @@
         <v>1</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B47" s="16">
         <v>25</v>
@@ -4738,19 +4733,19 @@
         <v>4</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G47" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="F47" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="G47" s="17" t="s">
+      <c r="H47" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="H47" s="15" t="s">
-        <v>264</v>
-      </c>
       <c r="I47" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J47" s="16">
         <v>25</v>
@@ -4778,7 +4773,7 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
@@ -4787,12 +4782,12 @@
         <v>0</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15">
       <c r="A48" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B48" s="16">
         <v>25</v>
@@ -4804,19 +4799,19 @@
         <v>29</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J48" s="16">
         <v>25</v>
@@ -4848,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T48" s="16">
         <v>0</v>
@@ -4857,12 +4852,12 @@
         <v>0</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B49" s="16">
         <v>26</v>
@@ -4874,19 +4869,19 @@
         <v>4</v>
       </c>
       <c r="E49" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="F49" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H49" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="I49" s="15" t="s">
         <v>271</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>272</v>
       </c>
       <c r="J49" s="16">
         <v>26</v>
@@ -4928,12 +4923,12 @@
         <v>1</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B50" s="16">
         <v>26</v>
@@ -4945,19 +4940,19 @@
         <v>29</v>
       </c>
       <c r="E50" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="G50" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G50" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H50" s="15" t="s">
+      <c r="I50" s="15" t="s">
         <v>275</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>276</v>
       </c>
       <c r="J50" s="16">
         <v>26</v>
@@ -4990,7 +4985,7 @@
         <v>1</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="T50" s="16">
         <v>0</v>
@@ -4999,12 +4994,12 @@
         <v>0</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B51" s="16">
         <v>27</v>
@@ -5016,19 +5011,19 @@
         <v>4</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F51" s="15" t="s">
         <v>278</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>279</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H51" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="I51" s="15" t="s">
         <v>280</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>281</v>
       </c>
       <c r="J51" s="16">
         <v>27</v>
@@ -5070,12 +5065,12 @@
         <v>1</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B52" s="16">
         <v>27</v>
@@ -5087,19 +5082,19 @@
         <v>29</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>282</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>283</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H52" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="I52" s="15" t="s">
         <v>284</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>285</v>
       </c>
       <c r="J52" s="16">
         <v>27</v>
@@ -5131,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="S52" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T52" s="16">
         <v>0</v>
@@ -5140,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -5167,24 +5162,24 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>286</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>287</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5206,14 +5201,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5228,14 +5223,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5250,14 +5245,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -5272,36 +5267,36 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="5">
         <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5316,36 +5311,36 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8">
         <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5360,24 +5355,24 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11">
         <v>37</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1">
@@ -5385,41 +5380,41 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
         <v>39</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
@@ -5527,7 +5522,7 @@
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
       <c r="C25" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>

</xml_diff>

<commit_message>
gazi directory setting and ne
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="331">
   <si>
     <t>operator</t>
   </si>
@@ -998,6 +998,21 @@
   </si>
   <si>
     <t>g:\telcobright\vault\resources\cdr\btcl\tdm\Mohakhali</t>
+  </si>
+  <si>
+    <t>btcl_SheraBangla</t>
+  </si>
+  <si>
+    <t>asdfasadf</t>
+  </si>
+  <si>
+    <t>g:\telcobright\vault\resources\cdr\btcl\tdm\SBN</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Vault.SBN</t>
   </si>
 </sst>
 </file>
@@ -1475,11 +1490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V52"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1489,6 +1504,7 @@
     <col min="5" max="5" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="14.140625" customWidth="1"/>
@@ -3049,7 +3065,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>4</v>
@@ -3110,48 +3126,46 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:22" s="32" customFormat="1" ht="15">
+      <c r="A24" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="27">
         <v>12</v>
       </c>
-      <c r="C24" s="16">
-        <v>1</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="27">
+        <v>2</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="34" t="s">
-        <v>324</v>
-      </c>
+      <c r="E24" s="26"/>
       <c r="F24" s="15" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="15" t="s">
-        <v>144</v>
+      <c r="H24" s="26" t="s">
+        <v>327</v>
       </c>
       <c r="I24" s="35" t="s">
-        <v>325</v>
-      </c>
-      <c r="J24" s="16">
+        <v>328</v>
+      </c>
+      <c r="J24" s="27">
         <v>12</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="29">
         <v>68</v>
       </c>
-      <c r="L24" s="20" t="s">
-        <v>322</v>
+      <c r="L24" s="30" t="s">
+        <v>329</v>
       </c>
       <c r="M24" s="21" t="str">
-        <f t="array" ref="M24">INDEX(Sheet2!$E$2:$F$21,MATCH(G24,Sheet2!$F$2:F43,0),1)</f>
+        <f t="array" ref="M24">INDEX(Sheet2!$E$2:$F$21,MATCH(G24,Sheet2!$F$2:F42,0),1)</f>
         <v>.dat</v>
       </c>
-      <c r="N24" s="15" t="s">
+      <c r="N24" s="26" t="s">
         <v>27</v>
       </c>
       <c r="O24" s="16">
@@ -3160,76 +3174,74 @@
       <c r="P24" s="16">
         <v>0</v>
       </c>
-      <c r="Q24" s="16">
-        <v>1</v>
-      </c>
-      <c r="R24" s="16">
+      <c r="Q24" s="27">
+        <v>1</v>
+      </c>
+      <c r="R24" s="27">
         <v>1</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="T24" s="16">
+        <v>330</v>
+      </c>
+      <c r="T24" s="27">
         <v>0</v>
       </c>
       <c r="U24" s="16">
         <v>0</v>
       </c>
-      <c r="V24" s="15" t="s">
+      <c r="V24" s="26" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15">
       <c r="A25" s="15" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B25" s="16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C25" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>146</v>
+        <v>29</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>324</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>147</v>
+        <v>321</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>325</v>
       </c>
       <c r="J25" s="16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K25" s="19">
-        <f t="array" ref="K25">INDEX(Sheet2!$H$2:$I$21,MATCH(G25,Sheet2!$I$2:I29,0),1)</f>
-        <v>25</v>
-      </c>
-      <c r="L25" s="20" t="str">
-        <f t="array" ref="L25">INDEX(Sheet2!$B$2:$C$21,MATCH(G25,Sheet2!$C$2:C44,0),1)</f>
-        <v>esdr</v>
+        <v>68</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>322</v>
       </c>
       <c r="M25" s="21" t="str">
-        <f t="array" ref="M25">INDEX(Sheet2!$E$2:$F$21,MATCH(G25,Sheet2!$F$2:F44,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M25">INDEX(Sheet2!$E$2:$F$21,MATCH(G25,Sheet2!$F$2:F43,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N25" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O25" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="16">
         <v>1</v>
@@ -3238,16 +3250,16 @@
         <v>1</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>150</v>
+        <v>323</v>
       </c>
       <c r="T25" s="16">
         <v>0</v>
       </c>
       <c r="U25" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15">
@@ -3258,48 +3270,49 @@
         <v>15</v>
       </c>
       <c r="C26" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J26" s="16">
         <v>15</v>
       </c>
       <c r="K26" s="19">
-        <f t="array" ref="K26">INDEX(Sheet2!$H$2:$I$21,MATCH(G26,Sheet2!$I$2:I30,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>314</v>
+        <f t="array" ref="K26">INDEX(Sheet2!$H$2:$I$21,MATCH(G26,Sheet2!$I$2:I29,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L26" s="20" t="str">
+        <f t="array" ref="L26">INDEX(Sheet2!$B$2:$C$21,MATCH(G26,Sheet2!$C$2:C44,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M26" s="21" t="str">
-        <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F45,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F44,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N26" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="16">
         <v>1</v>
@@ -3308,13 +3321,13 @@
         <v>1</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>303</v>
+        <v>150</v>
       </c>
       <c r="T26" s="16">
         <v>0</v>
       </c>
       <c r="U26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="15" t="s">
         <v>145</v>
@@ -3322,55 +3335,54 @@
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B27" s="16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="16">
+        <v>1</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27" s="16">
+        <v>15</v>
+      </c>
+      <c r="K27" s="19">
+        <f t="array" ref="K27">INDEX(Sheet2!$H$2:$I$21,MATCH(G27,Sheet2!$I$2:I30,0),1)</f>
         <v>3</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="J27" s="16">
-        <v>16</v>
-      </c>
-      <c r="K27" s="19">
-        <f t="array" ref="K27">INDEX(Sheet2!$H$2:$I$21,MATCH(G27,Sheet2!$I$2:I31,0),1)</f>
-        <v>25</v>
-      </c>
-      <c r="L27" s="20" t="str">
-        <f t="array" ref="L27">INDEX(Sheet2!$B$2:$C$21,MATCH(G27,Sheet2!$C$2:C46,0),1)</f>
-        <v>esdr</v>
+      <c r="L27" s="20" t="s">
+        <v>314</v>
       </c>
       <c r="M27" s="21" t="str">
-        <f t="array" ref="M27">INDEX(Sheet2!$E$2:$F$21,MATCH(G27,Sheet2!$F$2:F46,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M27">INDEX(Sheet2!$E$2:$F$21,MATCH(G27,Sheet2!$F$2:F45,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N27" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="16">
         <v>1</v>
@@ -3379,16 +3391,16 @@
         <v>1</v>
       </c>
       <c r="S27" s="15" t="s">
-        <v>67</v>
+        <v>303</v>
       </c>
       <c r="T27" s="16">
         <v>0</v>
       </c>
       <c r="U27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15">
@@ -3399,48 +3411,49 @@
         <v>16</v>
       </c>
       <c r="C28" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J28" s="16">
         <v>16</v>
       </c>
       <c r="K28" s="19">
-        <f t="array" ref="K28">INDEX(Sheet2!$H$2:$I$21,MATCH(G28,Sheet2!$I$2:I32,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L28" s="20" t="s">
-        <v>308</v>
+        <f t="array" ref="K28">INDEX(Sheet2!$H$2:$I$21,MATCH(G28,Sheet2!$I$2:I31,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L28" s="20" t="str">
+        <f t="array" ref="L28">INDEX(Sheet2!$B$2:$C$21,MATCH(G28,Sheet2!$C$2:C46,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M28" s="21" t="str">
-        <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F47,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F46,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N28" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O28" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="16">
         <v>1</v>
@@ -3449,13 +3462,13 @@
         <v>1</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>302</v>
+        <v>67</v>
       </c>
       <c r="T28" s="16">
         <v>0</v>
       </c>
       <c r="U28" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="15" t="s">
         <v>155</v>
@@ -3463,43 +3476,45 @@
     </row>
     <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B29" s="16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="16">
         <v>2</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J29" s="16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K29" s="19">
-        <v>56</v>
-      </c>
-      <c r="L29" s="20">
-        <v>0</v>
-      </c>
-      <c r="M29" s="21" t="s">
-        <v>318</v>
+        <f t="array" ref="K29">INDEX(Sheet2!$H$2:$I$21,MATCH(G29,Sheet2!$I$2:I32,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="M29" s="21" t="str">
+        <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F47,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N29" s="15" t="s">
         <v>27</v>
@@ -3517,7 +3532,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3526,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15">
@@ -3537,48 +3552,46 @@
         <v>17</v>
       </c>
       <c r="C30" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J30" s="16">
         <v>17</v>
       </c>
       <c r="K30" s="19">
-        <f t="array" ref="K30">INDEX(Sheet2!$H$2:$I$21,MATCH(G30,Sheet2!$I$2:I34,0),1)</f>
-        <v>17</v>
-      </c>
-      <c r="L30" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="M30" s="21" t="str">
-        <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G30,Sheet2!$F$2:F49,0),1)</f>
-        <v>.DAT</v>
+        <v>56</v>
+      </c>
+      <c r="L30" s="20">
+        <v>0</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>318</v>
       </c>
       <c r="N30" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O30" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="16">
         <v>1</v>
@@ -3587,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="T30" s="16">
         <v>0</v>
@@ -3601,54 +3614,54 @@
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B31" s="16">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J31" s="16">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K31" s="19">
-        <v>40</v>
-      </c>
-      <c r="L31" s="20" t="str">
-        <f t="array" ref="L31">INDEX(Sheet2!$B$2:$C$21,MATCH(G31,Sheet2!$C$2:C50,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="K31">INDEX(Sheet2!$H$2:$I$21,MATCH(G31,Sheet2!$I$2:I34,0),1)</f>
+        <v>17</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>301</v>
       </c>
       <c r="M31" s="21" t="str">
-        <f t="array" ref="M31">INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F50,0),1)</f>
-        <v>.txt</v>
+        <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F49,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N31" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O31" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="16">
         <v>1</v>
@@ -3657,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>28</v>
+        <v>300</v>
       </c>
       <c r="T31" s="16">
         <v>0</v>
@@ -3666,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
@@ -3677,49 +3690,48 @@
         <v>18</v>
       </c>
       <c r="C32" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J32" s="16">
         <v>18</v>
       </c>
       <c r="K32" s="19">
-        <f t="array" ref="K32">INDEX(Sheet2!$H$2:$I$21,MATCH(G32,Sheet2!$I$2:I36,0),1)</f>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L32" s="20" t="str">
-        <f t="array" ref="L32">INDEX(Sheet2!$B$2:$C$21,MATCH(G32,Sheet2!$C$2:C51,0),1)</f>
-        <v>VCDR</v>
+        <f t="array" ref="L32">INDEX(Sheet2!$B$2:$C$21,MATCH(G32,Sheet2!$C$2:C50,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M32" s="21" t="str">
-        <f t="array" ref="M32">INDEX(Sheet2!$E$2:$F$21,MATCH(G32,Sheet2!$F$2:F51,0),1)</f>
-        <v>.gz</v>
+        <f t="array" ref="M32">INDEX(Sheet2!$E$2:$F$21,MATCH(G32,Sheet2!$F$2:F50,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N32" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="16">
         <v>1</v>
@@ -3728,13 +3740,13 @@
         <v>1</v>
       </c>
       <c r="S32" s="15" t="s">
-        <v>183</v>
+        <v>28</v>
       </c>
       <c r="T32" s="16">
         <v>0</v>
       </c>
       <c r="U32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V32" s="15" t="s">
         <v>174</v>
@@ -3748,40 +3760,40 @@
         <v>18</v>
       </c>
       <c r="C33" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="J33" s="16">
         <v>18</v>
       </c>
       <c r="K33" s="19">
-        <f t="array" ref="K33">INDEX(Sheet2!$H$2:$I$21,MATCH(G33,Sheet2!$I$2:I37,0),1)</f>
-        <v>37</v>
+        <f t="array" ref="K33">INDEX(Sheet2!$H$2:$I$21,MATCH(G33,Sheet2!$I$2:I36,0),1)</f>
+        <v>31</v>
       </c>
       <c r="L33" s="20" t="str">
-        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C52,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C51,0),1)</f>
+        <v>VCDR</v>
       </c>
       <c r="M33" s="21" t="str">
-        <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F52,0),1)</f>
-        <v>.log</v>
+        <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F51,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N33" s="15" t="s">
         <v>27</v>
@@ -3799,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
@@ -3813,46 +3825,46 @@
     </row>
     <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B34" s="16">
-        <v>19</v>
-      </c>
-      <c r="C34" s="25">
         <v>18</v>
       </c>
+      <c r="C34" s="16">
+        <v>2</v>
+      </c>
       <c r="D34" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="J34" s="16">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K34" s="19">
-        <f t="array" ref="K34">INDEX(Sheet2!$H$2:$I$21,MATCH(G34,Sheet2!$I$2:I38,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K34">INDEX(Sheet2!$H$2:$I$21,MATCH(G34,Sheet2!$I$2:I37,0),1)</f>
+        <v>37</v>
       </c>
       <c r="L34" s="20" t="str">
-        <f t="array" ref="L34">INDEX(Sheet2!$B$2:$C$21,MATCH(G34,Sheet2!$C$2:C53,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L34">INDEX(Sheet2!$B$2:$C$21,MATCH(G34,Sheet2!$C$2:C52,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M34" s="21" t="str">
-        <f t="array" ref="M34">INDEX(Sheet2!$E$2:$F$21,MATCH(G34,Sheet2!$F$2:F53,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M34">INDEX(Sheet2!$E$2:$F$21,MATCH(G34,Sheet2!$F$2:F52,0),1)</f>
+        <v>.log</v>
       </c>
       <c r="N34" s="15" t="s">
         <v>27</v>
@@ -3870,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="T34" s="16">
         <v>0</v>
@@ -3879,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
@@ -3890,48 +3902,49 @@
         <v>19</v>
       </c>
       <c r="C35" s="25">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J35" s="16">
         <v>19</v>
       </c>
       <c r="K35" s="19">
-        <f t="array" ref="K35">INDEX(Sheet2!$H$2:$I$21,MATCH(G35,Sheet2!$I$2:I39,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L35" s="20" t="s">
-        <v>298</v>
+        <f t="array" ref="K35">INDEX(Sheet2!$H$2:$I$21,MATCH(G35,Sheet2!$I$2:I38,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L35" s="20" t="str">
+        <f t="array" ref="L35">INDEX(Sheet2!$B$2:$C$21,MATCH(G35,Sheet2!$C$2:C53,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M35" s="21" t="str">
-        <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F54,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F53,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="O35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q35" s="16">
         <v>1</v>
@@ -3940,13 +3953,13 @@
         <v>1</v>
       </c>
       <c r="S35" s="15" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="T35" s="16">
         <v>0</v>
       </c>
       <c r="U35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V35" s="15" t="s">
         <v>189</v>
@@ -3954,55 +3967,54 @@
     </row>
     <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B36" s="16">
-        <v>20</v>
-      </c>
-      <c r="C36" s="16">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="C36" s="25">
+        <v>8</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="J36" s="16">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="19">
-        <f t="array" ref="K36">INDEX(Sheet2!$H$2:$I$21,MATCH(G36,Sheet2!$I$2:I40,0),1)</f>
-        <v>28</v>
-      </c>
-      <c r="L36" s="20" t="str">
-        <f t="array" ref="L36">INDEX(Sheet2!$B$2:$C$21,MATCH(G36,Sheet2!$C$2:C55,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="K36">INDEX(Sheet2!$H$2:$I$21,MATCH(G36,Sheet2!$I$2:I39,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>298</v>
       </c>
       <c r="M36" s="21" t="str">
-        <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F55,0),1)</f>
-        <v>.csv</v>
+        <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F54,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="O36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="16">
         <v>1</v>
@@ -4011,16 +4023,16 @@
         <v>1</v>
       </c>
       <c r="S36" s="15" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
       <c r="T36" s="16">
         <v>0</v>
       </c>
       <c r="U36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15">
@@ -4031,48 +4043,49 @@
         <v>20</v>
       </c>
       <c r="C37" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J37" s="16">
         <v>20</v>
       </c>
       <c r="K37" s="19">
-        <f t="array" ref="K37">INDEX(Sheet2!$H$2:$I$21,MATCH(G37,Sheet2!$I$2:I41,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L37" s="20" t="s">
-        <v>290</v>
+        <f t="array" ref="K37">INDEX(Sheet2!$H$2:$I$21,MATCH(G37,Sheet2!$I$2:I40,0),1)</f>
+        <v>28</v>
+      </c>
+      <c r="L37" s="20" t="str">
+        <f t="array" ref="L37">INDEX(Sheet2!$B$2:$C$21,MATCH(G37,Sheet2!$C$2:C55,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M37" s="21" t="str">
-        <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F56,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F55,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N37" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="16">
         <v>1</v>
@@ -4081,13 +4094,13 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
       </c>
       <c r="U37" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V37" s="15" t="s">
         <v>198</v>
@@ -4095,55 +4108,54 @@
     </row>
     <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B38" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J38" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K38" s="19">
-        <f t="array" ref="K38">INDEX(Sheet2!$H$2:$I$21,MATCH(G38,Sheet2!$I$2:I42,0),1)</f>
-        <v>25</v>
-      </c>
-      <c r="L38" s="20" t="str">
-        <f t="array" ref="L38">INDEX(Sheet2!$B$2:$C$21,MATCH(G38,Sheet2!$C$2:C57,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="K38">INDEX(Sheet2!$H$2:$I$21,MATCH(G38,Sheet2!$I$2:I41,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>290</v>
       </c>
       <c r="M38" s="21" t="str">
-        <f t="array" ref="M38">INDEX(Sheet2!$E$2:$F$21,MATCH(G38,Sheet2!$F$2:F57,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M38">INDEX(Sheet2!$E$2:$F$21,MATCH(G38,Sheet2!$F$2:F56,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N38" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O38" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="16">
         <v>1</v>
@@ -4152,7 +4164,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>213</v>
+        <v>303</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4161,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="V38" s="15" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
@@ -4172,49 +4184,49 @@
         <v>21</v>
       </c>
       <c r="C39" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J39" s="16">
         <v>21</v>
       </c>
       <c r="K39" s="19">
-        <f t="array" ref="K39">INDEX(Sheet2!$H$2:$I$21,MATCH(G39,Sheet2!$I$2:I43,0),1)</f>
-        <v>3</v>
+        <f t="array" ref="K39">INDEX(Sheet2!$H$2:$I$21,MATCH(G39,Sheet2!$I$2:I42,0),1)</f>
+        <v>25</v>
       </c>
       <c r="L39" s="20" t="str">
-        <f t="array" ref="L39">INDEX(Sheet2!$B$2:$C$21,MATCH(G39,Sheet2!$C$2:C58,0),1)</f>
-        <v>b</v>
+        <f t="array" ref="L39">INDEX(Sheet2!$B$2:$C$21,MATCH(G39,Sheet2!$C$2:C57,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M39" s="21" t="str">
-        <f t="array" ref="M39">INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F58,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M39">INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F57,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N39" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O39" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q39" s="16">
         <v>1</v>
@@ -4223,7 +4235,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>303</v>
+        <v>213</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
@@ -4237,55 +4249,55 @@
     </row>
     <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B40" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" s="16">
+        <v>1</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40" s="16">
+        <v>21</v>
+      </c>
+      <c r="K40" s="19">
+        <f t="array" ref="K40">INDEX(Sheet2!$H$2:$I$21,MATCH(G40,Sheet2!$I$2:I43,0),1)</f>
         <v>3</v>
       </c>
-      <c r="D40" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="J40" s="16">
-        <v>22</v>
-      </c>
-      <c r="K40" s="19">
-        <f t="array" ref="K40">INDEX(Sheet2!$H$2:$I$21,MATCH(G40,Sheet2!$I$2:I44,0),1)</f>
-        <v>25</v>
-      </c>
       <c r="L40" s="20" t="str">
-        <f t="array" ref="L40">INDEX(Sheet2!$B$2:$C$21,MATCH(G40,Sheet2!$C$2:C59,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L40">INDEX(Sheet2!$B$2:$C$21,MATCH(G40,Sheet2!$C$2:C58,0),1)</f>
+        <v>b</v>
       </c>
       <c r="M40" s="21" t="str">
-        <f t="array" ref="M40">INDEX(Sheet2!$E$2:$F$21,MATCH(G40,Sheet2!$F$2:F59,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M40">INDEX(Sheet2!$E$2:$F$21,MATCH(G40,Sheet2!$F$2:F58,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N40" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O40" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="16">
         <v>1</v>
@@ -4294,16 +4306,16 @@
         <v>1</v>
       </c>
       <c r="S40" s="15" t="s">
-        <v>223</v>
+        <v>303</v>
       </c>
       <c r="T40" s="16">
         <v>0</v>
       </c>
       <c r="U40" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15">
@@ -4314,40 +4326,40 @@
         <v>22</v>
       </c>
       <c r="C41" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J41" s="16">
         <v>22</v>
       </c>
       <c r="K41" s="19">
-        <f t="array" ref="K41">INDEX(Sheet2!$H$2:$I$21,MATCH(G41,Sheet2!$I$2:I45,0),1)</f>
-        <v>3</v>
+        <f t="array" ref="K41">INDEX(Sheet2!$H$2:$I$21,MATCH(G41,Sheet2!$I$2:I44,0),1)</f>
+        <v>25</v>
       </c>
       <c r="L41" s="20" t="str">
-        <f t="array" ref="L41">INDEX(Sheet2!$B$2:$C$21,MATCH(G41,Sheet2!$C$2:C60,0),1)</f>
-        <v>b</v>
+        <f t="array" ref="L41">INDEX(Sheet2!$B$2:$C$21,MATCH(G41,Sheet2!$C$2:C59,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M41" s="21" t="str">
-        <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F60,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F59,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N41" s="15" t="s">
         <v>27</v>
@@ -4365,7 +4377,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
@@ -4385,42 +4397,42 @@
         <v>22</v>
       </c>
       <c r="C42" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J42" s="16">
         <v>22</v>
       </c>
       <c r="K42" s="19">
-        <f t="array" ref="K42">INDEX(Sheet2!$H$2:$I$21,MATCH(G42,Sheet2!$I$2:I46,0),1)</f>
-        <v>37</v>
+        <f t="array" ref="K42">INDEX(Sheet2!$H$2:$I$21,MATCH(G42,Sheet2!$I$2:I45,0),1)</f>
+        <v>3</v>
       </c>
       <c r="L42" s="20" t="str">
-        <f t="array" ref="L42">INDEX(Sheet2!$B$2:$C$21,MATCH(G42,Sheet2!$C$2:C61,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="L42">INDEX(Sheet2!$B$2:$C$21,MATCH(G42,Sheet2!$C$2:C60,0),1)</f>
+        <v>b</v>
       </c>
       <c r="M42" s="21" t="str">
-        <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F61,0),1)</f>
-        <v>.log</v>
-      </c>
-      <c r="N42" s="18" t="s">
+        <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F60,0),1)</f>
+        <v>.dat</v>
+      </c>
+      <c r="N42" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O42" s="16">
@@ -4436,7 +4448,7 @@
         <v>1</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
@@ -4450,48 +4462,48 @@
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B43" s="16">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" s="16">
         <v>2</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J43" s="16">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K43" s="19">
-        <f t="array" ref="K43">INDEX(Sheet2!$H$2:$I$21,MATCH(G43,Sheet2!$I$2:I47,0),1)</f>
-        <v>28</v>
+        <f t="array" ref="K43">INDEX(Sheet2!$H$2:$I$21,MATCH(G43,Sheet2!$I$2:I46,0),1)</f>
+        <v>37</v>
       </c>
       <c r="L43" s="20" t="str">
-        <f t="array" ref="L43">INDEX(Sheet2!$B$2:$C$21,MATCH(G43,Sheet2!$C$2:C62,0),1)</f>
+        <f t="array" ref="L43">INDEX(Sheet2!$B$2:$C$21,MATCH(G43,Sheet2!$C$2:C61,0),1)</f>
         <v>cdr</v>
       </c>
       <c r="M43" s="21" t="str">
-        <f t="array" ref="M43">INDEX(Sheet2!$E$2:$F$21,MATCH(G43,Sheet2!$F$2:F62,0),1)</f>
-        <v>.csv</v>
-      </c>
-      <c r="N43" s="15" t="s">
+        <f t="array" ref="M43">INDEX(Sheet2!$E$2:$F$21,MATCH(G43,Sheet2!$F$2:F61,0),1)</f>
+        <v>.log</v>
+      </c>
+      <c r="N43" s="18" t="s">
         <v>27</v>
       </c>
       <c r="O43" s="16">
@@ -4507,7 +4519,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>112</v>
+        <v>233</v>
       </c>
       <c r="T43" s="16">
         <v>0</v>
@@ -4516,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15">
@@ -4527,40 +4539,40 @@
         <v>23</v>
       </c>
       <c r="C44" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>241</v>
+        <v>24</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="J44" s="16">
         <v>23</v>
       </c>
       <c r="K44" s="19">
-        <f t="array" ref="K44">INDEX(Sheet2!$H$2:$I$21,MATCH(G44,Sheet2!$I$2:I48,0),1)</f>
-        <v>36</v>
+        <f t="array" ref="K44">INDEX(Sheet2!$H$2:$I$21,MATCH(G44,Sheet2!$I$2:I47,0),1)</f>
+        <v>28</v>
       </c>
       <c r="L44" s="20" t="str">
-        <f t="array" ref="L44">INDEX(Sheet2!$B$2:$C$21,MATCH(G44,Sheet2!$C$2:C63,0),1)</f>
-        <v>CF</v>
+        <f t="array" ref="L44">INDEX(Sheet2!$B$2:$C$21,MATCH(G44,Sheet2!$C$2:C62,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M44" s="21" t="str">
-        <f t="array" ref="M44">INDEX(Sheet2!$E$2:$F$21,MATCH(G44,Sheet2!$F$2:F63,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M44">INDEX(Sheet2!$E$2:$F$21,MATCH(G44,Sheet2!$F$2:F62,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N44" s="15" t="s">
         <v>27</v>
@@ -4578,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>244</v>
+        <v>112</v>
       </c>
       <c r="T44" s="16">
         <v>0</v>
@@ -4592,46 +4604,46 @@
     </row>
     <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B45" s="16">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>40</v>
+        <v>241</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J45" s="16">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K45" s="19">
-        <f t="array" ref="K45">INDEX(Sheet2!$H$2:$I$21,MATCH(G45,Sheet2!$I$2:I49,0),1)</f>
-        <v>27</v>
+        <f t="array" ref="K45">INDEX(Sheet2!$H$2:$I$21,MATCH(G45,Sheet2!$I$2:I48,0),1)</f>
+        <v>36</v>
       </c>
       <c r="L45" s="20" t="str">
-        <f t="array" ref="L45">INDEX(Sheet2!$B$2:$C$21,MATCH(G45,Sheet2!$C$2:C64,0),1)</f>
-        <v>sdr</v>
+        <f t="array" ref="L45">INDEX(Sheet2!$B$2:$C$21,MATCH(G45,Sheet2!$C$2:C63,0),1)</f>
+        <v>CF</v>
       </c>
       <c r="M45" s="21" t="str">
-        <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F64,0),1)</f>
-        <v>.gz</v>
+        <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F63,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N45" s="15" t="s">
         <v>27</v>
@@ -4649,16 +4661,16 @@
         <v>1</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="T45" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45" s="16">
         <v>1</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="15">
@@ -4669,40 +4681,40 @@
         <v>24</v>
       </c>
       <c r="C46" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J46" s="16">
         <v>24</v>
       </c>
       <c r="K46" s="19">
-        <f t="array" ref="K46">INDEX(Sheet2!$H$2:$I$21,MATCH(G46,Sheet2!$I$2:I50,0),1)</f>
-        <v>36</v>
+        <f t="array" ref="K46">INDEX(Sheet2!$H$2:$I$21,MATCH(G46,Sheet2!$I$2:I49,0),1)</f>
+        <v>27</v>
       </c>
       <c r="L46" s="20" t="str">
-        <f t="array" ref="L46">INDEX(Sheet2!$B$2:$C$21,MATCH(G46,Sheet2!$C$2:C65,0),1)</f>
-        <v>CF</v>
+        <f t="array" ref="L46">INDEX(Sheet2!$B$2:$C$21,MATCH(G46,Sheet2!$C$2:C64,0),1)</f>
+        <v>sdr</v>
       </c>
       <c r="M46" s="21" t="str">
-        <f t="array" ref="M46">INDEX(Sheet2!$E$2:$F$21,MATCH(G46,Sheet2!$F$2:F65,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M46">INDEX(Sheet2!$E$2:$F$21,MATCH(G46,Sheet2!$F$2:F64,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N46" s="15" t="s">
         <v>27</v>
@@ -4720,10 +4732,10 @@
         <v>1</v>
       </c>
       <c r="S46" s="15" t="s">
-        <v>36</v>
+        <v>250</v>
       </c>
       <c r="T46" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46" s="16">
         <v>1</v>
@@ -4734,50 +4746,55 @@
     </row>
     <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>309</v>
+        <v>245</v>
       </c>
       <c r="B47" s="16">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C47" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>310</v>
+        <v>252</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>312</v>
+        <v>254</v>
       </c>
       <c r="J47" s="16">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K47" s="19">
-        <v>55</v>
-      </c>
-      <c r="L47" s="20">
-        <v>2</v>
-      </c>
-      <c r="M47" s="21"/>
+        <f t="array" ref="K47">INDEX(Sheet2!$H$2:$I$21,MATCH(G47,Sheet2!$I$2:I50,0),1)</f>
+        <v>36</v>
+      </c>
+      <c r="L47" s="20" t="str">
+        <f t="array" ref="L47">INDEX(Sheet2!$B$2:$C$21,MATCH(G47,Sheet2!$C$2:C65,0),1)</f>
+        <v>CF</v>
+      </c>
+      <c r="M47" s="21" t="str">
+        <f t="array" ref="M47">INDEX(Sheet2!$E$2:$F$21,MATCH(G47,Sheet2!$F$2:F65,0),1)</f>
+        <v>.DAT</v>
+      </c>
       <c r="N47" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q47" s="16">
         <v>1</v>
@@ -4786,16 +4803,16 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>316</v>
+        <v>36</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
       </c>
       <c r="U47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15">
@@ -4806,40 +4823,36 @@
         <v>25</v>
       </c>
       <c r="C48" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J48" s="16">
         <v>25</v>
       </c>
       <c r="K48" s="19">
-        <f t="array" ref="K48">INDEX(Sheet2!$H$2:$I$21,MATCH(G48,Sheet2!$I$2:I52,0),1)</f>
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="L48" s="20">
         <v>2</v>
       </c>
-      <c r="M48" s="21" t="str">
-        <f t="array" ref="M48">INDEX(Sheet2!$E$2:$F$21,MATCH(G48,Sheet2!$F$2:F67,0),1)</f>
-        <v>.dat</v>
-      </c>
+      <c r="M48" s="21"/>
       <c r="N48" s="15" t="s">
         <v>27</v>
       </c>
@@ -4856,7 +4869,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="T48" s="16">
         <v>0</v>
@@ -4870,55 +4883,54 @@
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>262</v>
+        <v>309</v>
       </c>
       <c r="B49" s="16">
-        <v>26</v>
-      </c>
-      <c r="C49" s="25">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="C49" s="16">
+        <v>1</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>266</v>
+        <v>313</v>
       </c>
       <c r="J49" s="16">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K49" s="19">
-        <f t="array" ref="K49">INDEX(Sheet2!$H$2:$I$21,MATCH(G49,Sheet2!$I$2:I53,0),1)</f>
-        <v>27</v>
-      </c>
-      <c r="L49" s="20" t="str">
-        <f t="array" ref="L49">INDEX(Sheet2!$B$2:$C$21,MATCH(G49,Sheet2!$C$2:C68,0),1)</f>
-        <v>sdr</v>
+        <f t="array" ref="K49">INDEX(Sheet2!$H$2:$I$21,MATCH(G49,Sheet2!$I$2:I52,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L49" s="20">
+        <v>2</v>
       </c>
       <c r="M49" s="21" t="str">
-        <f t="array" ref="M49">INDEX(Sheet2!$E$2:$F$21,MATCH(G49,Sheet2!$F$2:F68,0),1)</f>
-        <v>.gz</v>
+        <f t="array" ref="M49">INDEX(Sheet2!$E$2:$F$21,MATCH(G49,Sheet2!$F$2:F67,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N49" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O49" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P49" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q49" s="16">
         <v>1</v>
@@ -4927,16 +4939,16 @@
         <v>1</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>43</v>
+        <v>302</v>
       </c>
       <c r="T49" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
@@ -4947,49 +4959,49 @@
         <v>26</v>
       </c>
       <c r="C50" s="25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J50" s="16">
         <v>26</v>
       </c>
       <c r="K50" s="19">
-        <f t="array" ref="K50">INDEX(Sheet2!$H$2:$I$21,MATCH(G50,Sheet2!$I$2:I54,0),1)</f>
-        <v>17</v>
+        <f t="array" ref="K50">INDEX(Sheet2!$H$2:$I$21,MATCH(G50,Sheet2!$I$2:I53,0),1)</f>
+        <v>27</v>
       </c>
       <c r="L50" s="20" t="str">
-        <f t="array" ref="L50">INDEX(Sheet2!$B$2:$C$21,MATCH(G50,Sheet2!$C$2:C69,0),1)</f>
-        <v>ICX</v>
+        <f t="array" ref="L50">INDEX(Sheet2!$B$2:$C$21,MATCH(G50,Sheet2!$C$2:C68,0),1)</f>
+        <v>sdr</v>
       </c>
       <c r="M50" s="21" t="str">
-        <f t="array" ref="M50">INDEX(Sheet2!$E$2:$F$21,MATCH(G50,Sheet2!$F$2:F69,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M50">INDEX(Sheet2!$E$2:$F$21,MATCH(G50,Sheet2!$F$2:F68,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N50" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="16">
         <v>1</v>
@@ -4998,13 +5010,13 @@
         <v>1</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>299</v>
+        <v>43</v>
       </c>
       <c r="T50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="15" t="s">
         <v>262</v>
@@ -5012,55 +5024,55 @@
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B51" s="16">
-        <v>27</v>
-      </c>
-      <c r="C51" s="16">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="C51" s="25">
+        <v>9</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J51" s="16">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K51" s="19">
-        <f t="array" ref="K51">INDEX(Sheet2!$H$2:$I$21,MATCH(G51,Sheet2!$I$2:I55,0),1)</f>
-        <v>28</v>
+        <f t="array" ref="K51">INDEX(Sheet2!$H$2:$I$21,MATCH(G51,Sheet2!$I$2:I54,0),1)</f>
+        <v>17</v>
       </c>
       <c r="L51" s="20" t="str">
-        <f t="array" ref="L51">INDEX(Sheet2!$B$2:$C$21,MATCH(G51,Sheet2!$C$2:C70,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="L51">INDEX(Sheet2!$B$2:$C$21,MATCH(G51,Sheet2!$C$2:C69,0),1)</f>
+        <v>ICX</v>
       </c>
       <c r="M51" s="21" t="str">
-        <f t="array" ref="M51">INDEX(Sheet2!$E$2:$F$21,MATCH(G51,Sheet2!$F$2:F70,0),1)</f>
-        <v>.csv</v>
+        <f t="array" ref="M51">INDEX(Sheet2!$E$2:$F$21,MATCH(G51,Sheet2!$F$2:F69,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N51" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O51" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P51" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="16">
         <v>1</v>
@@ -5069,16 +5081,16 @@
         <v>1</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>49</v>
+        <v>299</v>
       </c>
       <c r="T51" s="16">
         <v>0</v>
       </c>
       <c r="U51" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
@@ -5089,65 +5101,136 @@
         <v>27</v>
       </c>
       <c r="C52" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J52" s="16">
         <v>27</v>
       </c>
       <c r="K52" s="19">
-        <f t="array" ref="K52">INDEX(Sheet2!$H$2:$I$21,MATCH(G52,Sheet2!$I$2:I56,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L52" s="33">
-        <v>2</v>
+        <f t="array" ref="K52">INDEX(Sheet2!$H$2:$I$21,MATCH(G52,Sheet2!$I$2:I55,0),1)</f>
+        <v>28</v>
+      </c>
+      <c r="L52" s="20" t="str">
+        <f t="array" ref="L52">INDEX(Sheet2!$B$2:$C$21,MATCH(G52,Sheet2!$C$2:C70,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M52" s="21" t="str">
-        <f t="array" ref="M52">INDEX(Sheet2!$E$2:$F$21,MATCH(G52,Sheet2!$F$2:F71,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M52">INDEX(Sheet2!$E$2:$F$21,MATCH(G52,Sheet2!$F$2:F70,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N52" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O52" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P52" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" s="16">
         <v>1</v>
       </c>
       <c r="R52" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="T52" s="16">
+        <v>0</v>
+      </c>
+      <c r="U52" s="16">
+        <v>1</v>
+      </c>
+      <c r="V52" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="15">
+      <c r="A53" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B53" s="16">
+        <v>27</v>
+      </c>
+      <c r="C53" s="16">
+        <v>1</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="J53" s="16">
+        <v>27</v>
+      </c>
+      <c r="K53" s="19">
+        <f t="array" ref="K53">INDEX(Sheet2!$H$2:$I$21,MATCH(G53,Sheet2!$I$2:I56,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L53" s="33">
+        <v>2</v>
+      </c>
+      <c r="M53" s="21" t="str">
+        <f t="array" ref="M53">INDEX(Sheet2!$E$2:$F$21,MATCH(G53,Sheet2!$F$2:F71,0),1)</f>
+        <v>.dat</v>
+      </c>
+      <c r="N53" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O53" s="16">
+        <v>0</v>
+      </c>
+      <c r="P53" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="16">
+        <v>1</v>
+      </c>
+      <c r="R53" s="16">
+        <v>0</v>
+      </c>
+      <c r="S53" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="T52" s="16">
-        <v>0</v>
-      </c>
-      <c r="U52" s="16">
-        <v>0</v>
-      </c>
-      <c r="V52" s="15" t="s">
+      <c r="T53" s="16">
+        <v>0</v>
+      </c>
+      <c r="U53" s="16">
+        <v>0</v>
+      </c>
+      <c r="V53" s="15" t="s">
         <v>271</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nokia Siemens Decoder added
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sftproot\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="332">
   <si>
     <t>operator</t>
   </si>
@@ -784,9 +784,6 @@
     <t>b07G7uf$Rt24</t>
   </si>
   <si>
-    <t>j:\telcobright\vault\resources\cdr\mothertelecom\tdm</t>
-  </si>
-  <si>
     <t>telePlusNetwork</t>
   </si>
   <si>
@@ -1013,6 +1010,12 @@
   </si>
   <si>
     <t>Vault.SBN</t>
+  </si>
+  <si>
+    <t>e:\telcobright\vault\resources\cdr\mothertelecom\tdm</t>
+  </si>
+  <si>
+    <t>vault.Nokia</t>
   </si>
 </sst>
 </file>
@@ -1492,9 +1495,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1714,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1856,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="T5" s="16">
         <v>0</v>
@@ -1974,7 +1977,7 @@
         <v>49</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="15" t="s">
@@ -2134,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T9" s="16">
         <v>0</v>
@@ -2251,7 +2254,7 @@
         <v>70</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M11" s="21"/>
       <c r="N11" s="15" t="s">
@@ -2317,7 +2320,7 @@
         <v>57</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M12" s="21" t="str">
         <f t="array" ref="M12">INDEX(Sheet2!$E$2:$F$21,MATCH(G12,Sheet2!$F$2:F31,0),1)</f>
@@ -2600,7 +2603,7 @@
         <v>17</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M16" s="21" t="str">
         <f t="array" ref="M16">INDEX(Sheet2!$E$2:$F$21,MATCH(G16,Sheet2!$F$2:F35,0),1)</f>
@@ -3023,7 +3026,7 @@
         <v>68</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M22" s="21" t="str">
         <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F41,0),1)</f>
@@ -3045,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T22" s="16">
         <v>0</v>
@@ -3141,16 +3144,16 @@
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H24" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="I24" s="35" t="s">
         <v>327</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>328</v>
       </c>
       <c r="J24" s="27">
         <v>12</v>
@@ -3159,7 +3162,7 @@
         <v>68</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M24" s="21" t="str">
         <f t="array" ref="M24">INDEX(Sheet2!$E$2:$F$21,MATCH(G24,Sheet2!$F$2:F42,0),1)</f>
@@ -3181,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T24" s="27">
         <v>0</v>
@@ -3207,10 +3210,10 @@
         <v>29</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>46</v>
@@ -3219,7 +3222,7 @@
         <v>144</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J25" s="16">
         <v>12</v>
@@ -3228,7 +3231,7 @@
         <v>68</v>
       </c>
       <c r="L25" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M25" s="21" t="str">
         <f t="array" ref="M25">INDEX(Sheet2!$E$2:$F$21,MATCH(G25,Sheet2!$F$2:F43,0),1)</f>
@@ -3250,7 +3253,7 @@
         <v>1</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T25" s="16">
         <v>0</v>
@@ -3369,7 +3372,7 @@
         <v>3</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M27" s="21" t="str">
         <f t="array" ref="M27">INDEX(Sheet2!$E$2:$F$21,MATCH(G27,Sheet2!$F$2:F45,0),1)</f>
@@ -3391,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="S27" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T27" s="16">
         <v>0</v>
@@ -3510,7 +3513,7 @@
         <v>3</v>
       </c>
       <c r="L29" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M29" s="21" t="str">
         <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F47,0),1)</f>
@@ -3532,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3582,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N30" s="15" t="s">
         <v>27</v>
@@ -3600,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="T30" s="16">
         <v>0</v>
@@ -3648,7 +3651,7 @@
         <v>17</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M31" s="21" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F49,0),1)</f>
@@ -3670,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="T31" s="16">
         <v>0</v>
@@ -4001,7 +4004,7 @@
         <v>3</v>
       </c>
       <c r="L36" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M36" s="21" t="str">
         <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F54,0),1)</f>
@@ -4142,7 +4145,7 @@
         <v>3</v>
       </c>
       <c r="L38" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M38" s="21" t="str">
         <f t="array" ref="M38">INDEX(Sheet2!$E$2:$F$21,MATCH(G38,Sheet2!$F$2:F56,0),1)</f>
@@ -4164,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4306,7 +4309,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T40" s="16">
         <v>0</v>
@@ -4770,18 +4773,16 @@
         <v>253</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="J47" s="16">
         <v>24</v>
       </c>
       <c r="K47" s="19">
-        <f t="array" ref="K47">INDEX(Sheet2!$H$2:$I$21,MATCH(G47,Sheet2!$I$2:I50,0),1)</f>
-        <v>36</v>
-      </c>
-      <c r="L47" s="20" t="str">
-        <f t="array" ref="L47">INDEX(Sheet2!$B$2:$C$21,MATCH(G47,Sheet2!$C$2:C65,0),1)</f>
-        <v>CF</v>
+        <v>74</v>
+      </c>
+      <c r="L47" s="20" t="s">
+        <v>328</v>
       </c>
       <c r="M47" s="21" t="str">
         <f t="array" ref="M47">INDEX(Sheet2!$E$2:$F$21,MATCH(G47,Sheet2!$F$2:F65,0),1)</f>
@@ -4791,10 +4792,10 @@
         <v>27</v>
       </c>
       <c r="O47" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="16">
         <v>1</v>
@@ -4803,13 +4804,13 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>36</v>
+        <v>331</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
       </c>
       <c r="U47" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V47" s="15" t="s">
         <v>245</v>
@@ -4817,7 +4818,7 @@
     </row>
     <row r="48" spans="1:22" ht="15">
       <c r="A48" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B48" s="16">
         <v>25</v>
@@ -4829,19 +4830,19 @@
         <v>4</v>
       </c>
       <c r="E48" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F48" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="G48" s="17" t="s">
+      <c r="H48" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="H48" s="15" t="s">
-        <v>258</v>
-      </c>
       <c r="I48" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J48" s="16">
         <v>25</v>
@@ -4869,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T48" s="16">
         <v>0</v>
@@ -4878,12 +4879,12 @@
         <v>0</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B49" s="16">
         <v>25</v>
@@ -4895,19 +4896,19 @@
         <v>29</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J49" s="16">
         <v>25</v>
@@ -4939,7 +4940,7 @@
         <v>1</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T49" s="16">
         <v>0</v>
@@ -4948,12 +4949,12 @@
         <v>0</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B50" s="16">
         <v>26</v>
@@ -4965,19 +4966,19 @@
         <v>4</v>
       </c>
       <c r="E50" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>263</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>264</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H50" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="I50" s="15" t="s">
         <v>265</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>266</v>
       </c>
       <c r="J50" s="16">
         <v>26</v>
@@ -5019,12 +5020,12 @@
         <v>1</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B51" s="16">
         <v>26</v>
@@ -5036,19 +5037,19 @@
         <v>29</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F51" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>268</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>104</v>
       </c>
       <c r="H51" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="I51" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="J51" s="16">
         <v>26</v>
@@ -5081,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T51" s="16">
         <v>0</v>
@@ -5090,12 +5091,12 @@
         <v>0</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B52" s="16">
         <v>27</v>
@@ -5107,19 +5108,19 @@
         <v>4</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>272</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>273</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H52" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="I52" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="J52" s="16">
         <v>27</v>
@@ -5161,12 +5162,12 @@
         <v>1</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15">
       <c r="A53" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B53" s="16">
         <v>27</v>
@@ -5178,19 +5179,19 @@
         <v>29</v>
       </c>
       <c r="E53" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>276</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>277</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H53" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="I53" s="15" t="s">
         <v>278</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>279</v>
       </c>
       <c r="J53" s="16">
         <v>27</v>
@@ -5222,7 +5223,7 @@
         <v>0</v>
       </c>
       <c r="S53" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T53" s="16">
         <v>0</v>
@@ -5231,7 +5232,7 @@
         <v>0</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5258,24 +5259,24 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>281</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5297,14 +5298,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5319,14 +5320,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5341,14 +5342,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -5363,14 +5364,14 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>104</v>
@@ -5385,14 +5386,14 @@
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5407,14 +5408,14 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>241</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>241</v>
@@ -5429,14 +5430,14 @@
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5451,14 +5452,14 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>83</v>
@@ -5476,31 +5477,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>167</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>167</v>
@@ -5618,7 +5619,7 @@
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
       <c r="C25" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>

</xml_diff>

<commit_message>
added cataleya bangla cas
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -190,9 +190,6 @@
     <t>d:\telcobright\vault\resources\cdr\bangla\ip</t>
   </si>
   <si>
-    <t>banglaicx_10.255.200.13_CATALEYA</t>
-  </si>
-  <si>
     <t>10.154.150.13</t>
   </si>
   <si>
@@ -1016,6 +1013,9 @@
   </si>
   <si>
     <t>vault.Nokia</t>
+  </si>
+  <si>
+    <t>Vault.Cataleya</t>
   </si>
 </sst>
 </file>
@@ -1496,8 +1496,8 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1731,55 +1731,54 @@
     </row>
     <row r="4" spans="1:22" ht="15">
       <c r="A4" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B4" s="16">
+        <v>3</v>
+      </c>
+      <c r="C4" s="16">
         <v>2</v>
-      </c>
-      <c r="C4" s="16">
-        <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="J4" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" s="19">
-        <f t="array" ref="K4">INDEX(Sheet2!$H$2:$I$21,MATCH(G4,Sheet2!$I$2:I8,0),1)</f>
+        <v>690</v>
+      </c>
+      <c r="L4" s="20" t="str">
+        <f t="array" ref="L4">INDEX(Sheet2!$B$2:$C$21,MATCH(G4,Sheet2!$C$2:C25,0),1)</f>
+        <v>esdr</v>
+      </c>
+      <c r="M4" s="21" t="str">
+        <f t="array" ref="M4">INDEX(Sheet2!$E$2:$F$21,MATCH(G4,Sheet2!$F$2:F25,0),1)</f>
+        <v>.txt</v>
+      </c>
+      <c r="N4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="20" t="str">
-        <f t="array" ref="L4">INDEX(Sheet2!$B$2:$C$21,MATCH(G4,Sheet2!$C$2:C23,0),1)</f>
-        <v>sdr</v>
-      </c>
-      <c r="M4" s="21" t="str">
-        <f t="array" ref="M4">INDEX(Sheet2!$E$2:$F$21,MATCH(G4,Sheet2!$F$2:F23,0),1)</f>
-        <v>.gz</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="O4" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="16">
         <v>1</v>
@@ -1788,61 +1787,56 @@
         <v>1</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>43</v>
+        <v>331</v>
       </c>
       <c r="T4" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="16">
         <v>0</v>
       </c>
       <c r="V4" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15">
       <c r="A5" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B5" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="J5" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5" s="19">
-        <f t="array" ref="K5">INDEX(Sheet2!$H$2:$I$21,MATCH(G5,Sheet2!$I$2:I9,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L5" s="20" t="str">
-        <f t="array" ref="L5">INDEX(Sheet2!$B$2:$C$21,MATCH(G5,Sheet2!$C$2:C24,0),1)</f>
-        <v>b</v>
-      </c>
-      <c r="M5" s="21" t="str">
-        <f t="array" ref="M5">INDEX(Sheet2!$E$2:$F$21,MATCH(G5,Sheet2!$F$2:F24,0),1)</f>
-        <v>.dat</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="M5" s="21"/>
       <c r="N5" s="15" t="s">
         <v>27</v>
       </c>
@@ -1859,63 +1853,63 @@
         <v>1</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>303</v>
+        <v>60</v>
       </c>
       <c r="T5" s="16">
         <v>0</v>
       </c>
       <c r="U5" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15">
       <c r="A6" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B6" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="16">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J6" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="19">
-        <f t="array" ref="K6">INDEX(Sheet2!$H$2:$I$21,MATCH(G6,Sheet2!$I$2:I10,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K6">INDEX(Sheet2!$H$2:$I$21,MATCH(G6,Sheet2!$I$2:I8,0),1)</f>
+        <v>27</v>
       </c>
       <c r="L6" s="20" t="str">
-        <f t="array" ref="L6">INDEX(Sheet2!$B$2:$C$21,MATCH(G6,Sheet2!$C$2:C25,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L6">INDEX(Sheet2!$B$2:$C$21,MATCH(G6,Sheet2!$C$2:C23,0),1)</f>
+        <v>sdr</v>
       </c>
       <c r="M6" s="21" t="str">
-        <f t="array" ref="M6">INDEX(Sheet2!$E$2:$F$21,MATCH(G6,Sheet2!$F$2:F25,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M6">INDEX(Sheet2!$E$2:$F$21,MATCH(G6,Sheet2!$F$2:F23,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="O6" s="16">
         <v>1</v>
@@ -1930,56 +1924,61 @@
         <v>1</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="T6" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="16">
         <v>0</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15">
       <c r="A7" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B7" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="16">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J7" s="16">
+        <v>2</v>
+      </c>
+      <c r="K7" s="19">
+        <f t="array" ref="K7">INDEX(Sheet2!$H$2:$I$21,MATCH(G7,Sheet2!$I$2:I9,0),1)</f>
         <v>3</v>
       </c>
-      <c r="K7" s="19">
-        <v>49</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="M7" s="21"/>
+      <c r="L7" s="20" t="str">
+        <f t="array" ref="L7">INDEX(Sheet2!$B$2:$C$21,MATCH(G7,Sheet2!$C$2:C24,0),1)</f>
+        <v>b</v>
+      </c>
+      <c r="M7" s="21" t="str">
+        <f t="array" ref="M7">INDEX(Sheet2!$E$2:$F$21,MATCH(G7,Sheet2!$F$2:F24,0),1)</f>
+        <v>.dat</v>
+      </c>
       <c r="N7" s="15" t="s">
         <v>27</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>61</v>
+        <v>302</v>
       </c>
       <c r="T7" s="16">
         <v>0</v>
@@ -2005,12 +2004,12 @@
         <v>0</v>
       </c>
       <c r="V7" s="15" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15">
       <c r="A8" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="16">
         <v>4</v>
@@ -2022,19 +2021,19 @@
         <v>4</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="J8" s="16">
         <v>4</v>
@@ -2066,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T8" s="16">
         <v>1</v>
@@ -2075,12 +2074,12 @@
         <v>1</v>
       </c>
       <c r="V8" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15">
       <c r="A9" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="16">
         <v>4</v>
@@ -2092,19 +2091,19 @@
         <v>29</v>
       </c>
       <c r="E9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="J9" s="16">
         <v>4</v>
@@ -2137,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T9" s="16">
         <v>0</v>
@@ -2146,52 +2145,51 @@
         <v>0</v>
       </c>
       <c r="V9" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15">
-      <c r="A10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="16">
-        <v>6</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="A10" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="27">
+        <v>12</v>
+      </c>
+      <c r="C10" s="27">
         <v>3</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="16">
-        <v>6</v>
-      </c>
-      <c r="K10" s="19">
-        <v>32</v>
-      </c>
-      <c r="L10" s="20" t="str">
-        <f t="array" ref="L10">INDEX(Sheet2!$B$2:$C$21,MATCH(G10,Sheet2!$C$2:C29,0),1)</f>
-        <v>esdr</v>
-      </c>
-      <c r="M10" s="21" t="str">
-        <f t="array" ref="M10">INDEX(Sheet2!$E$2:$F$21,MATCH(G10,Sheet2!$F$2:F29,0),1)</f>
-        <v>.txt</v>
-      </c>
-      <c r="N10" s="15" t="s">
+      <c r="E10" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="27">
+        <v>12</v>
+      </c>
+      <c r="K10" s="29" t="e">
+        <f t="array" ref="K10">INDEX(Sheet2!$H$2:$I$21,MATCH(G10,Sheet2!$I$2:I27,0),1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L10" s="30" t="e">
+        <f t="array" ref="L10">INDEX(Sheet2!$B$2:$C$21,MATCH(G10,Sheet2!$C$2:C42,0),1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M10" s="31" t="e">
+        <f t="array" ref="M10">INDEX(Sheet2!$E$2:$F$21,MATCH(G10,Sheet2!$F$2:F42,0),1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N10" s="26" t="s">
         <v>27</v>
       </c>
       <c r="O10" s="16">
@@ -2200,131 +2198,132 @@
       <c r="P10" s="16">
         <v>1</v>
       </c>
-      <c r="Q10" s="16">
-        <v>1</v>
-      </c>
-      <c r="R10" s="16">
-        <v>1</v>
-      </c>
-      <c r="S10" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" s="16">
+      <c r="Q10" s="27">
+        <v>1</v>
+      </c>
+      <c r="R10" s="27">
+        <v>1</v>
+      </c>
+      <c r="S10" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="T10" s="27">
         <v>0</v>
       </c>
       <c r="U10" s="16">
-        <v>0</v>
-      </c>
-      <c r="V10" s="15" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="V10" s="26" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15">
-      <c r="A11" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="16">
-        <v>6</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="A11" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="27">
+        <v>12</v>
+      </c>
+      <c r="C11" s="27">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="E11" s="26"/>
       <c r="F11" s="15" t="s">
-        <v>78</v>
+        <v>324</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="16">
-        <v>6</v>
-      </c>
-      <c r="K11" s="19">
-        <v>70</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="J11" s="27">
+        <v>12</v>
+      </c>
+      <c r="K11" s="29">
+        <v>68</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="M11" s="21" t="str">
+        <f t="array" ref="M11">INDEX(Sheet2!$E$2:$F$21,MATCH(G11,Sheet2!$F$2:F42,0),1)</f>
+        <v>.dat</v>
+      </c>
+      <c r="N11" s="26" t="s">
         <v>27</v>
       </c>
       <c r="O11" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>1</v>
-      </c>
-      <c r="R11" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>1</v>
+      </c>
+      <c r="R11" s="27">
         <v>1</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="T11" s="16">
+        <v>328</v>
+      </c>
+      <c r="T11" s="27">
         <v>0</v>
       </c>
       <c r="U11" s="16">
-        <v>1</v>
-      </c>
-      <c r="V11" s="15" t="s">
-        <v>72</v>
+        <v>0</v>
+      </c>
+      <c r="V11" s="26" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15">
       <c r="A12" s="15" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="B12" s="16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C12" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>81</v>
+      <c r="E12" s="34" t="s">
+        <v>322</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>82</v>
+        <v>319</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>85</v>
+        <v>143</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>323</v>
       </c>
       <c r="J12" s="16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K12" s="19">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M12" s="21" t="str">
-        <f t="array" ref="M12">INDEX(Sheet2!$E$2:$F$21,MATCH(G12,Sheet2!$F$2:F31,0),1)</f>
-        <v>.log</v>
+        <f t="array" ref="M12">INDEX(Sheet2!$E$2:$F$21,MATCH(G12,Sheet2!$F$2:F43,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N12" s="15" t="s">
         <v>27</v>
@@ -2342,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>233</v>
+        <v>321</v>
       </c>
       <c r="T12" s="16">
         <v>0</v>
@@ -2351,60 +2350,59 @@
         <v>0</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15">
       <c r="A13" s="15" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="B13" s="16">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>90</v>
+        <v>177</v>
       </c>
       <c r="J13" s="16">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="K13" s="19">
-        <f t="array" ref="K13">INDEX(Sheet2!$H$2:$I$21,MATCH(G13,Sheet2!$I$2:I17,0),1)</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="L13" s="20" t="str">
-        <f t="array" ref="L13">INDEX(Sheet2!$B$2:$C$21,MATCH(G13,Sheet2!$C$2:C32,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="L13">INDEX(Sheet2!$B$2:$C$21,MATCH(G13,Sheet2!$C$2:C50,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M13" s="21" t="str">
-        <f t="array" ref="M13">INDEX(Sheet2!$E$2:$F$21,MATCH(G13,Sheet2!$F$2:F32,0),1)</f>
-        <v>.csv</v>
+        <f t="array" ref="M13">INDEX(Sheet2!$E$2:$F$21,MATCH(G13,Sheet2!$F$2:F50,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N13" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="16">
         <v>1</v>
@@ -2413,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="T13" s="16">
         <v>0</v>
@@ -2422,15 +2420,15 @@
         <v>0</v>
       </c>
       <c r="V13" s="15" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15">
       <c r="A14" s="15" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="B14" s="16">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C14" s="16">
         <v>1</v>
@@ -2439,34 +2437,34 @@
         <v>29</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>93</v>
+        <v>179</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="J14" s="16">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="K14" s="19">
-        <f t="array" ref="K14">INDEX(Sheet2!$H$2:$I$21,MATCH(G14,Sheet2!$I$2:I18,0),1)</f>
-        <v>3</v>
+        <f t="array" ref="K14">INDEX(Sheet2!$H$2:$I$21,MATCH(G14,Sheet2!$I$2:I36,0),1)</f>
+        <v>31</v>
       </c>
       <c r="L14" s="20" t="str">
-        <f t="array" ref="L14">INDEX(Sheet2!$B$2:$C$21,MATCH(G14,Sheet2!$C$2:C33,0),1)</f>
-        <v>b</v>
+        <f t="array" ref="L14">INDEX(Sheet2!$B$2:$C$21,MATCH(G14,Sheet2!$C$2:C51,0),1)</f>
+        <v>VCDR</v>
       </c>
       <c r="M14" s="21" t="str">
-        <f t="array" ref="M14">INDEX(Sheet2!$E$2:$F$21,MATCH(G14,Sheet2!$F$2:F33,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M14">INDEX(Sheet2!$E$2:$F$21,MATCH(G14,Sheet2!$F$2:F51,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>27</v>
@@ -2484,60 +2482,60 @@
         <v>1</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="T14" s="16">
         <v>0</v>
       </c>
       <c r="U14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="15" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15">
       <c r="A15" s="15" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="B15" s="16">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="16">
         <v>2</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="J15" s="16">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="K15" s="19">
-        <f t="array" ref="K15">INDEX(Sheet2!$H$2:$I$21,MATCH(G15,Sheet2!$I$2:I19,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K15">INDEX(Sheet2!$H$2:$I$21,MATCH(G15,Sheet2!$I$2:I37,0),1)</f>
+        <v>37</v>
       </c>
       <c r="L15" s="20" t="str">
-        <f t="array" ref="L15">INDEX(Sheet2!$B$2:$C$21,MATCH(G15,Sheet2!$C$2:C34,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L15">INDEX(Sheet2!$B$2:$C$21,MATCH(G15,Sheet2!$C$2:C52,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M15" s="21" t="str">
-        <f t="array" ref="M15">INDEX(Sheet2!$E$2:$F$21,MATCH(G15,Sheet2!$F$2:F34,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M15">INDEX(Sheet2!$E$2:$F$21,MATCH(G15,Sheet2!$F$2:F52,0),1)</f>
+        <v>.log</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>27</v>
@@ -2555,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="T15" s="16">
         <v>0</v>
@@ -2564,59 +2562,59 @@
         <v>1</v>
       </c>
       <c r="V15" s="15" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
       <c r="A16" s="15" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B16" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="J16" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K16" s="19">
-        <f t="array" ref="K16">INDEX(Sheet2!$H$2:$I$21,MATCH(G16,Sheet2!$I$2:I20,0),1)</f>
-        <v>17</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>306</v>
+        <v>32</v>
+      </c>
+      <c r="L16" s="20" t="str">
+        <f t="array" ref="L16">INDEX(Sheet2!$B$2:$C$21,MATCH(G16,Sheet2!$C$2:C29,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M16" s="21" t="str">
-        <f t="array" ref="M16">INDEX(Sheet2!$E$2:$F$21,MATCH(G16,Sheet2!$F$2:F35,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M16">INDEX(Sheet2!$E$2:$F$21,MATCH(G16,Sheet2!$F$2:F29,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="16">
         <v>1</v>
@@ -2625,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="T16" s="16">
         <v>0</v>
@@ -2634,51 +2632,47 @@
         <v>0</v>
       </c>
       <c r="V16" s="15" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
       <c r="A17" s="15" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B17" s="16">
-        <v>9</v>
-      </c>
-      <c r="C17" s="25">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="J17" s="16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K17" s="19">
-        <v>30</v>
-      </c>
-      <c r="L17" s="20" t="str">
-        <f t="array" ref="L17">INDEX(Sheet2!$B$2:$C$21,MATCH(G17,Sheet2!$C$2:C36,0),1)</f>
-        <v>esdr</v>
-      </c>
-      <c r="M17" s="21" t="str">
-        <f t="array" ref="M17">INDEX(Sheet2!$E$2:$F$21,MATCH(G17,Sheet2!$F$2:F36,0),1)</f>
-        <v>.txt</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="M17" s="21"/>
       <c r="N17" s="15" t="s">
         <v>27</v>
       </c>
@@ -2695,60 +2689,58 @@
         <v>1</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="T17" s="16">
         <v>0</v>
       </c>
       <c r="U17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="15" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
       <c r="A18" s="15" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B18" s="16">
-        <v>9</v>
-      </c>
-      <c r="C18" s="25">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="16">
+        <v>2</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="J18" s="16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K18" s="19">
-        <f t="array" ref="K18">INDEX(Sheet2!$H$2:$I$21,MATCH(G18,Sheet2!$I$2:I22,0),1)</f>
-        <v>17</v>
-      </c>
-      <c r="L18" s="20" t="str">
-        <f t="array" ref="L18">INDEX(Sheet2!$B$2:$C$21,MATCH(G18,Sheet2!$C$2:C37,0),1)</f>
-        <v>ICX</v>
+        <v>57</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="M18" s="21" t="str">
-        <f t="array" ref="M18">INDEX(Sheet2!$E$2:$F$21,MATCH(G18,Sheet2!$F$2:F37,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M18">INDEX(Sheet2!$E$2:$F$21,MATCH(G18,Sheet2!$F$2:F31,0),1)</f>
+        <v>.log</v>
       </c>
       <c r="N18" s="15" t="s">
         <v>27</v>
@@ -2766,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="T18" s="16">
         <v>0</v>
@@ -2775,15 +2767,15 @@
         <v>0</v>
       </c>
       <c r="V18" s="15" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15">
       <c r="A19" s="15" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B19" s="16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C19" s="16">
         <v>2</v>
@@ -2792,34 +2784,34 @@
         <v>4</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="J19" s="16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K19" s="19">
-        <f t="array" ref="K19">INDEX(Sheet2!$H$2:$I$21,MATCH(G19,Sheet2!$I$2:I23,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K19">INDEX(Sheet2!$H$2:$I$21,MATCH(G19,Sheet2!$I$2:I17,0),1)</f>
+        <v>28</v>
       </c>
       <c r="L19" s="20" t="str">
-        <f t="array" ref="L19">INDEX(Sheet2!$B$2:$C$21,MATCH(G19,Sheet2!$C$2:C38,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L19">INDEX(Sheet2!$B$2:$C$21,MATCH(G19,Sheet2!$C$2:C32,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M19" s="21" t="str">
-        <f t="array" ref="M19">INDEX(Sheet2!$E$2:$F$21,MATCH(G19,Sheet2!$F$2:F38,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M19">INDEX(Sheet2!$E$2:$F$21,MATCH(G19,Sheet2!$F$2:F32,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N19" s="15" t="s">
         <v>27</v>
@@ -2837,24 +2829,24 @@
         <v>1</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="T19" s="16">
         <v>0</v>
       </c>
       <c r="U19" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="15" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15">
       <c r="A20" s="15" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B20" s="16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20" s="16">
         <v>1</v>
@@ -2863,34 +2855,34 @@
         <v>29</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="J20" s="16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K20" s="19">
-        <f t="array" ref="K20">INDEX(Sheet2!$H$2:$I$21,MATCH(G20,Sheet2!$I$2:I24,0),1)</f>
-        <v>17</v>
+        <f t="array" ref="K20">INDEX(Sheet2!$H$2:$I$21,MATCH(G20,Sheet2!$I$2:I18,0),1)</f>
+        <v>3</v>
       </c>
       <c r="L20" s="20" t="str">
-        <f t="array" ref="L20">INDEX(Sheet2!$B$2:$C$21,MATCH(G20,Sheet2!$C$2:C39,0),1)</f>
-        <v>ICX</v>
+        <f t="array" ref="L20">INDEX(Sheet2!$B$2:$C$21,MATCH(G20,Sheet2!$C$2:C33,0),1)</f>
+        <v>b</v>
       </c>
       <c r="M20" s="21" t="str">
-        <f t="array" ref="M20">INDEX(Sheet2!$E$2:$F$21,MATCH(G20,Sheet2!$F$2:F39,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M20">INDEX(Sheet2!$E$2:$F$21,MATCH(G20,Sheet2!$F$2:F33,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N20" s="15" t="s">
         <v>27</v>
@@ -2908,24 +2900,24 @@
         <v>1</v>
       </c>
       <c r="S20" s="15" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="T20" s="16">
         <v>0</v>
       </c>
       <c r="U20" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="15" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15">
       <c r="A21" s="15" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="B21" s="16">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C21" s="16">
         <v>2</v>
@@ -2934,33 +2926,33 @@
         <v>4</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="J21" s="16">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K21" s="19">
-        <f t="array" ref="K21">INDEX(Sheet2!$H$2:$I$21,MATCH(G21,Sheet2!$I$2:I25,0),1)</f>
+        <f t="array" ref="K21">INDEX(Sheet2!$H$2:$I$21,MATCH(G21,Sheet2!$I$2:I19,0),1)</f>
         <v>25</v>
       </c>
       <c r="L21" s="20" t="str">
-        <f t="array" ref="L21">INDEX(Sheet2!$B$2:$C$21,MATCH(G21,Sheet2!$C$2:C40,0),1)</f>
+        <f t="array" ref="L21">INDEX(Sheet2!$B$2:$C$21,MATCH(G21,Sheet2!$C$2:C34,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M21" s="21" t="str">
-        <f t="array" ref="M21">INDEX(Sheet2!$E$2:$F$21,MATCH(G21,Sheet2!$F$2:F40,0),1)</f>
+        <f t="array" ref="M21">INDEX(Sheet2!$E$2:$F$21,MATCH(G21,Sheet2!$F$2:F34,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N21" s="15" t="s">
@@ -2979,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="T21" s="16">
         <v>0</v>
@@ -2988,15 +2980,15 @@
         <v>1</v>
       </c>
       <c r="V21" s="15" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15">
       <c r="A22" s="15" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="B22" s="16">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C22" s="16">
         <v>1</v>
@@ -3005,32 +2997,33 @@
         <v>29</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="J22" s="16">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K22" s="19">
-        <v>68</v>
+        <f t="array" ref="K22">INDEX(Sheet2!$H$2:$I$21,MATCH(G22,Sheet2!$I$2:I20,0),1)</f>
+        <v>17</v>
       </c>
       <c r="L22" s="20" t="s">
         <v>305</v>
       </c>
       <c r="M22" s="21" t="str">
-        <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F41,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F35,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N22" s="15" t="s">
         <v>27</v>
@@ -3048,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>302</v>
+        <v>116</v>
       </c>
       <c r="T22" s="16">
         <v>0</v>
@@ -3057,51 +3050,52 @@
         <v>0</v>
       </c>
       <c r="V22" s="15" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="32" customFormat="1" ht="15">
-      <c r="A23" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="27">
-        <v>12</v>
-      </c>
-      <c r="C23" s="27">
-        <v>3</v>
-      </c>
-      <c r="D23" s="26" t="s">
+      <c r="A23" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="16">
+        <v>9</v>
+      </c>
+      <c r="C23" s="25">
+        <v>18</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="I23" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="J23" s="27">
-        <v>12</v>
-      </c>
-      <c r="K23" s="29" t="e">
-        <f t="array" ref="K23">INDEX(Sheet2!$H$2:$I$21,MATCH(G23,Sheet2!$I$2:I27,0),1)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L23" s="30" t="e">
-        <f t="array" ref="L23">INDEX(Sheet2!$B$2:$C$21,MATCH(G23,Sheet2!$C$2:C42,0),1)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M23" s="31" t="e">
-        <f t="array" ref="M23">INDEX(Sheet2!$E$2:$F$21,MATCH(G23,Sheet2!$F$2:F42,0),1)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N23" s="26" t="s">
+      <c r="E23" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="16">
+        <v>9</v>
+      </c>
+      <c r="K23" s="19">
+        <v>30</v>
+      </c>
+      <c r="L23" s="20" t="str">
+        <f t="array" ref="L23">INDEX(Sheet2!$B$2:$C$21,MATCH(G23,Sheet2!$C$2:C36,0),1)</f>
+        <v>esdr</v>
+      </c>
+      <c r="M23" s="21" t="str">
+        <f t="array" ref="M23">INDEX(Sheet2!$E$2:$F$21,MATCH(G23,Sheet2!$F$2:F36,0),1)</f>
+        <v>.txt</v>
+      </c>
+      <c r="N23" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O23" s="16">
@@ -3110,65 +3104,69 @@
       <c r="P23" s="16">
         <v>1</v>
       </c>
-      <c r="Q23" s="27">
-        <v>1</v>
-      </c>
-      <c r="R23" s="27">
-        <v>1</v>
-      </c>
-      <c r="S23" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="T23" s="27">
+      <c r="Q23" s="16">
+        <v>1</v>
+      </c>
+      <c r="R23" s="16">
+        <v>1</v>
+      </c>
+      <c r="S23" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="T23" s="16">
         <v>0</v>
       </c>
       <c r="U23" s="16">
-        <v>1</v>
-      </c>
-      <c r="V23" s="26" t="s">
-        <v>138</v>
+        <v>0</v>
+      </c>
+      <c r="V23" s="15" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="32" customFormat="1" ht="15">
-      <c r="A24" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="27">
-        <v>12</v>
-      </c>
-      <c r="C24" s="27">
-        <v>2</v>
-      </c>
-      <c r="D24" s="26" t="s">
+      <c r="A24" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="16">
+        <v>9</v>
+      </c>
+      <c r="C24" s="25">
+        <v>7</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="26"/>
+      <c r="E24" s="15" t="s">
+        <v>112</v>
+      </c>
       <c r="F24" s="15" t="s">
-        <v>325</v>
+        <v>113</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>327</v>
-      </c>
-      <c r="J24" s="27">
-        <v>12</v>
-      </c>
-      <c r="K24" s="29">
-        <v>68</v>
-      </c>
-      <c r="L24" s="30" t="s">
-        <v>328</v>
+        <v>103</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="16">
+        <v>9</v>
+      </c>
+      <c r="K24" s="19">
+        <f t="array" ref="K24">INDEX(Sheet2!$H$2:$I$21,MATCH(G24,Sheet2!$I$2:I22,0),1)</f>
+        <v>17</v>
+      </c>
+      <c r="L24" s="20" t="str">
+        <f t="array" ref="L24">INDEX(Sheet2!$B$2:$C$21,MATCH(G24,Sheet2!$C$2:C37,0),1)</f>
+        <v>ICX</v>
       </c>
       <c r="M24" s="21" t="str">
-        <f t="array" ref="M24">INDEX(Sheet2!$E$2:$F$21,MATCH(G24,Sheet2!$F$2:F42,0),1)</f>
-        <v>.dat</v>
-      </c>
-      <c r="N24" s="26" t="s">
+        <f t="array" ref="M24">INDEX(Sheet2!$E$2:$F$21,MATCH(G24,Sheet2!$F$2:F37,0),1)</f>
+        <v>.DAT</v>
+      </c>
+      <c r="N24" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O24" s="16">
@@ -3177,74 +3175,76 @@
       <c r="P24" s="16">
         <v>0</v>
       </c>
-      <c r="Q24" s="27">
-        <v>1</v>
-      </c>
-      <c r="R24" s="27">
+      <c r="Q24" s="16">
+        <v>1</v>
+      </c>
+      <c r="R24" s="16">
         <v>1</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="T24" s="27">
+        <v>116</v>
+      </c>
+      <c r="T24" s="16">
         <v>0</v>
       </c>
       <c r="U24" s="16">
         <v>0</v>
       </c>
-      <c r="V24" s="26" t="s">
-        <v>138</v>
+      <c r="V24" s="15" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15">
       <c r="A25" s="15" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B25" s="16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C25" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>323</v>
+        <v>4</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>320</v>
+        <v>119</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" s="35" t="s">
-        <v>324</v>
+        <v>120</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="J25" s="16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K25" s="19">
-        <v>68</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>321</v>
+        <f t="array" ref="K25">INDEX(Sheet2!$H$2:$I$21,MATCH(G25,Sheet2!$I$2:I23,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L25" s="20" t="str">
+        <f t="array" ref="L25">INDEX(Sheet2!$B$2:$C$21,MATCH(G25,Sheet2!$C$2:C38,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M25" s="21" t="str">
-        <f t="array" ref="M25">INDEX(Sheet2!$E$2:$F$21,MATCH(G25,Sheet2!$F$2:F43,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M25">INDEX(Sheet2!$E$2:$F$21,MATCH(G25,Sheet2!$F$2:F38,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N25" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="16">
         <v>1</v>
@@ -3253,60 +3253,60 @@
         <v>1</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>322</v>
+        <v>122</v>
       </c>
       <c r="T25" s="16">
         <v>0</v>
       </c>
       <c r="U25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="15" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15">
       <c r="A26" s="15" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B26" s="16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C26" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="J26" s="16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K26" s="19">
-        <f t="array" ref="K26">INDEX(Sheet2!$H$2:$I$21,MATCH(G26,Sheet2!$I$2:I29,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K26">INDEX(Sheet2!$H$2:$I$21,MATCH(G26,Sheet2!$I$2:I24,0),1)</f>
+        <v>17</v>
       </c>
       <c r="L26" s="20" t="str">
-        <f t="array" ref="L26">INDEX(Sheet2!$B$2:$C$21,MATCH(G26,Sheet2!$C$2:C44,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L26">INDEX(Sheet2!$B$2:$C$21,MATCH(G26,Sheet2!$C$2:C39,0),1)</f>
+        <v>ICX</v>
       </c>
       <c r="M26" s="21" t="str">
-        <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F44,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M26">INDEX(Sheet2!$E$2:$F$21,MATCH(G26,Sheet2!$F$2:F39,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N26" s="15" t="s">
         <v>27</v>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="T26" s="16">
         <v>0</v>
@@ -3333,59 +3333,60 @@
         <v>1</v>
       </c>
       <c r="V26" s="15" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B27" s="16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C27" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="J27" s="16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K27" s="19">
-        <f t="array" ref="K27">INDEX(Sheet2!$H$2:$I$21,MATCH(G27,Sheet2!$I$2:I30,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L27" s="20" t="s">
-        <v>313</v>
+        <f t="array" ref="K27">INDEX(Sheet2!$H$2:$I$21,MATCH(G27,Sheet2!$I$2:I25,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L27" s="20" t="str">
+        <f t="array" ref="L27">INDEX(Sheet2!$B$2:$C$21,MATCH(G27,Sheet2!$C$2:C40,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M27" s="21" t="str">
-        <f t="array" ref="M27">INDEX(Sheet2!$E$2:$F$21,MATCH(G27,Sheet2!$F$2:F45,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M27">INDEX(Sheet2!$E$2:$F$21,MATCH(G27,Sheet2!$F$2:F40,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N27" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27" s="16">
         <v>1</v>
@@ -3394,69 +3395,67 @@
         <v>1</v>
       </c>
       <c r="S27" s="15" t="s">
-        <v>302</v>
+        <v>132</v>
       </c>
       <c r="T27" s="16">
         <v>0</v>
       </c>
       <c r="U27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15">
       <c r="A28" s="15" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B28" s="16">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C28" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="J28" s="16">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K28" s="19">
-        <f t="array" ref="K28">INDEX(Sheet2!$H$2:$I$21,MATCH(G28,Sheet2!$I$2:I31,0),1)</f>
-        <v>25</v>
-      </c>
-      <c r="L28" s="20" t="str">
-        <f t="array" ref="L28">INDEX(Sheet2!$B$2:$C$21,MATCH(G28,Sheet2!$C$2:C46,0),1)</f>
-        <v>esdr</v>
+        <v>68</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>304</v>
       </c>
       <c r="M28" s="21" t="str">
-        <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F46,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M28">INDEX(Sheet2!$E$2:$F$21,MATCH(G28,Sheet2!$F$2:F41,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N28" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O28" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="16">
         <v>1</v>
@@ -3465,68 +3464,69 @@
         <v>1</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>67</v>
+        <v>301</v>
       </c>
       <c r="T28" s="16">
         <v>0</v>
       </c>
       <c r="U28" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V28" s="15" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="B29" s="16">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C29" s="16">
         <v>2</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>160</v>
+        <v>245</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
       <c r="J29" s="16">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K29" s="19">
-        <f t="array" ref="K29">INDEX(Sheet2!$H$2:$I$21,MATCH(G29,Sheet2!$I$2:I32,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L29" s="20" t="s">
-        <v>307</v>
+        <f t="array" ref="K29">INDEX(Sheet2!$H$2:$I$21,MATCH(G29,Sheet2!$I$2:I49,0),1)</f>
+        <v>27</v>
+      </c>
+      <c r="L29" s="20" t="str">
+        <f t="array" ref="L29">INDEX(Sheet2!$B$2:$C$21,MATCH(G29,Sheet2!$C$2:C64,0),1)</f>
+        <v>sdr</v>
       </c>
       <c r="M29" s="21" t="str">
-        <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F47,0),1)</f>
-        <v>.dat</v>
+        <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F64,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N29" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="16">
         <v>1</v>
@@ -3535,57 +3535,58 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>301</v>
+        <v>249</v>
       </c>
       <c r="T29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29" s="15" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
-        <v>164</v>
+        <v>244</v>
       </c>
       <c r="B30" s="16">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C30" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>165</v>
+        <v>250</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>166</v>
+        <v>251</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>167</v>
+        <v>240</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>168</v>
+        <v>252</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>169</v>
+        <v>329</v>
       </c>
       <c r="J30" s="16">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K30" s="19">
-        <v>56</v>
-      </c>
-      <c r="L30" s="20">
-        <v>0</v>
-      </c>
-      <c r="M30" s="21" t="s">
-        <v>317</v>
+        <v>74</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="M30" s="21" t="str">
+        <f t="array" ref="M30">INDEX(Sheet2!$E$2:$F$21,MATCH(G30,Sheet2!$F$2:F65,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N30" s="15" t="s">
         <v>27</v>
@@ -3603,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="T30" s="16">
         <v>0</v>
@@ -3612,50 +3613,51 @@
         <v>0</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>164</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>164</v>
+        <v>233</v>
       </c>
       <c r="B31" s="16">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C31" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>172</v>
+        <v>236</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="J31" s="16">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K31" s="19">
-        <f t="array" ref="K31">INDEX(Sheet2!$H$2:$I$21,MATCH(G31,Sheet2!$I$2:I34,0),1)</f>
-        <v>17</v>
-      </c>
-      <c r="L31" s="20" t="s">
-        <v>300</v>
+        <f t="array" ref="K31">INDEX(Sheet2!$H$2:$I$21,MATCH(G31,Sheet2!$I$2:I47,0),1)</f>
+        <v>28</v>
+      </c>
+      <c r="L31" s="20" t="str">
+        <f t="array" ref="L31">INDEX(Sheet2!$B$2:$C$21,MATCH(G31,Sheet2!$C$2:C62,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M31" s="21" t="str">
-        <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F49,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M31">INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F62,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N31" s="15" t="s">
         <v>27</v>
@@ -3673,68 +3675,69 @@
         <v>1</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>299</v>
+        <v>111</v>
       </c>
       <c r="T31" s="16">
         <v>0</v>
       </c>
       <c r="U31" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>164</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
       <c r="A32" s="15" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
       <c r="B32" s="16">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C32" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>175</v>
+        <v>238</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>178</v>
+        <v>242</v>
       </c>
       <c r="J32" s="16">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K32" s="19">
-        <v>40</v>
+        <f t="array" ref="K32">INDEX(Sheet2!$H$2:$I$21,MATCH(G32,Sheet2!$I$2:I48,0),1)</f>
+        <v>36</v>
       </c>
       <c r="L32" s="20" t="str">
-        <f t="array" ref="L32">INDEX(Sheet2!$B$2:$C$21,MATCH(G32,Sheet2!$C$2:C50,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L32">INDEX(Sheet2!$B$2:$C$21,MATCH(G32,Sheet2!$C$2:C63,0),1)</f>
+        <v>CF</v>
       </c>
       <c r="M32" s="21" t="str">
-        <f t="array" ref="M32">INDEX(Sheet2!$E$2:$F$21,MATCH(G32,Sheet2!$F$2:F50,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M32">INDEX(Sheet2!$E$2:$F$21,MATCH(G32,Sheet2!$F$2:F63,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N32" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O32" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="16">
         <v>1</v>
@@ -3743,60 +3746,60 @@
         <v>1</v>
       </c>
       <c r="S32" s="15" t="s">
-        <v>28</v>
+        <v>243</v>
       </c>
       <c r="T32" s="16">
         <v>0</v>
       </c>
       <c r="U32" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15">
       <c r="A33" s="15" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B33" s="16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="J33" s="16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K33" s="19">
-        <f t="array" ref="K33">INDEX(Sheet2!$H$2:$I$21,MATCH(G33,Sheet2!$I$2:I36,0),1)</f>
-        <v>31</v>
+        <f t="array" ref="K33">INDEX(Sheet2!$H$2:$I$21,MATCH(G33,Sheet2!$I$2:I29,0),1)</f>
+        <v>25</v>
       </c>
       <c r="L33" s="20" t="str">
-        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C51,0),1)</f>
-        <v>VCDR</v>
+        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C44,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M33" s="21" t="str">
-        <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F51,0),1)</f>
-        <v>.gz</v>
+        <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F44,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N33" s="15" t="s">
         <v>27</v>
@@ -3814,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
@@ -3823,60 +3826,59 @@
         <v>1</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B34" s="16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C34" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="J34" s="16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K34" s="19">
-        <f t="array" ref="K34">INDEX(Sheet2!$H$2:$I$21,MATCH(G34,Sheet2!$I$2:I37,0),1)</f>
-        <v>37</v>
-      </c>
-      <c r="L34" s="20" t="str">
-        <f t="array" ref="L34">INDEX(Sheet2!$B$2:$C$21,MATCH(G34,Sheet2!$C$2:C52,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="K34">INDEX(Sheet2!$H$2:$I$21,MATCH(G34,Sheet2!$I$2:I30,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>312</v>
       </c>
       <c r="M34" s="21" t="str">
-        <f t="array" ref="M34">INDEX(Sheet2!$E$2:$F$21,MATCH(G34,Sheet2!$F$2:F52,0),1)</f>
-        <v>.log</v>
+        <f t="array" ref="M34">INDEX(Sheet2!$E$2:$F$21,MATCH(G34,Sheet2!$F$2:F45,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N34" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="16">
         <v>1</v>
@@ -3885,59 +3887,59 @@
         <v>1</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>188</v>
+        <v>301</v>
       </c>
       <c r="T34" s="16">
         <v>0</v>
       </c>
       <c r="U34" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34" s="15" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
       <c r="A35" s="15" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="B35" s="16">
-        <v>19</v>
-      </c>
-      <c r="C35" s="25">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C35" s="16">
+        <v>3</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="J35" s="16">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K35" s="19">
-        <f t="array" ref="K35">INDEX(Sheet2!$H$2:$I$21,MATCH(G35,Sheet2!$I$2:I38,0),1)</f>
+        <f t="array" ref="K35">INDEX(Sheet2!$H$2:$I$21,MATCH(G35,Sheet2!$I$2:I31,0),1)</f>
         <v>25</v>
       </c>
       <c r="L35" s="20" t="str">
-        <f t="array" ref="L35">INDEX(Sheet2!$B$2:$C$21,MATCH(G35,Sheet2!$C$2:C53,0),1)</f>
+        <f t="array" ref="L35">INDEX(Sheet2!$B$2:$C$21,MATCH(G35,Sheet2!$C$2:C46,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M35" s="21" t="str">
-        <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F53,0),1)</f>
+        <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F46,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N35" s="15" t="s">
@@ -3956,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="S35" s="15" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="T35" s="16">
         <v>0</v>
@@ -3965,53 +3967,53 @@
         <v>1</v>
       </c>
       <c r="V35" s="15" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="B36" s="16">
-        <v>19</v>
-      </c>
-      <c r="C36" s="25">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="C36" s="16">
+        <v>2</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="J36" s="16">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K36" s="19">
-        <f t="array" ref="K36">INDEX(Sheet2!$H$2:$I$21,MATCH(G36,Sheet2!$I$2:I39,0),1)</f>
+        <f t="array" ref="K36">INDEX(Sheet2!$H$2:$I$21,MATCH(G36,Sheet2!$I$2:I32,0),1)</f>
         <v>3</v>
       </c>
       <c r="L36" s="20" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="M36" s="21" t="str">
-        <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F54,0),1)</f>
+        <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F47,0),1)</f>
         <v>.dat</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="O36" s="16">
         <v>0</v>
@@ -4026,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="S36" s="15" t="s">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="T36" s="16">
         <v>0</v>
@@ -4035,15 +4037,15 @@
         <v>0</v>
       </c>
       <c r="V36" s="15" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15">
       <c r="A37" s="15" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B37" s="16">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C37" s="16">
         <v>2</v>
@@ -4052,43 +4054,40 @@
         <v>4</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="J37" s="16">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K37" s="19">
-        <f t="array" ref="K37">INDEX(Sheet2!$H$2:$I$21,MATCH(G37,Sheet2!$I$2:I40,0),1)</f>
-        <v>28</v>
-      </c>
-      <c r="L37" s="20" t="str">
-        <f t="array" ref="L37">INDEX(Sheet2!$B$2:$C$21,MATCH(G37,Sheet2!$C$2:C55,0),1)</f>
-        <v>cdr</v>
-      </c>
-      <c r="M37" s="21" t="str">
-        <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F55,0),1)</f>
-        <v>.csv</v>
+        <v>56</v>
+      </c>
+      <c r="L37" s="20">
+        <v>0</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>316</v>
       </c>
       <c r="N37" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="16">
         <v>1</v>
@@ -4097,24 +4096,24 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
       </c>
       <c r="U37" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V37" s="15" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B38" s="16">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C38" s="16">
         <v>1</v>
@@ -4123,42 +4122,42 @@
         <v>29</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="J38" s="16">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K38" s="19">
-        <f t="array" ref="K38">INDEX(Sheet2!$H$2:$I$21,MATCH(G38,Sheet2!$I$2:I41,0),1)</f>
-        <v>3</v>
+        <f t="array" ref="K38">INDEX(Sheet2!$H$2:$I$21,MATCH(G38,Sheet2!$I$2:I34,0),1)</f>
+        <v>17</v>
       </c>
       <c r="L38" s="20" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="M38" s="21" t="str">
-        <f t="array" ref="M38">INDEX(Sheet2!$E$2:$F$21,MATCH(G38,Sheet2!$F$2:F56,0),1)</f>
-        <v>.dat</v>
+        <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G38,Sheet2!$F$2:F49,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N38" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O38" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q38" s="16">
         <v>1</v>
@@ -4167,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4176,15 +4175,15 @@
         <v>0</v>
       </c>
       <c r="V38" s="15" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
       <c r="A39" s="15" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B39" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39" s="16">
         <v>2</v>
@@ -4193,34 +4192,34 @@
         <v>4</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="J39" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K39" s="19">
-        <f t="array" ref="K39">INDEX(Sheet2!$H$2:$I$21,MATCH(G39,Sheet2!$I$2:I42,0),1)</f>
-        <v>25</v>
+        <f t="array" ref="K39">INDEX(Sheet2!$H$2:$I$21,MATCH(G39,Sheet2!$I$2:I40,0),1)</f>
+        <v>28</v>
       </c>
       <c r="L39" s="20" t="str">
-        <f t="array" ref="L39">INDEX(Sheet2!$B$2:$C$21,MATCH(G39,Sheet2!$C$2:C57,0),1)</f>
-        <v>esdr</v>
+        <f t="array" ref="L39">INDEX(Sheet2!$B$2:$C$21,MATCH(G39,Sheet2!$C$2:C55,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M39" s="21" t="str">
-        <f t="array" ref="M39">INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F57,0),1)</f>
-        <v>.txt</v>
+        <f t="array" ref="M39">INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F55,0),1)</f>
+        <v>.csv</v>
       </c>
       <c r="N39" s="15" t="s">
         <v>27</v>
@@ -4238,24 +4237,24 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
       </c>
       <c r="U39" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V39" s="15" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B40" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40" s="16">
         <v>1</v>
@@ -4264,33 +4263,32 @@
         <v>29</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="J40" s="16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K40" s="19">
-        <f t="array" ref="K40">INDEX(Sheet2!$H$2:$I$21,MATCH(G40,Sheet2!$I$2:I43,0),1)</f>
+        <f t="array" ref="K40">INDEX(Sheet2!$H$2:$I$21,MATCH(G40,Sheet2!$I$2:I41,0),1)</f>
         <v>3</v>
       </c>
-      <c r="L40" s="20" t="str">
-        <f t="array" ref="L40">INDEX(Sheet2!$B$2:$C$21,MATCH(G40,Sheet2!$C$2:C58,0),1)</f>
-        <v>b</v>
+      <c r="L40" s="20" t="s">
+        <v>288</v>
       </c>
       <c r="M40" s="21" t="str">
-        <f t="array" ref="M40">INDEX(Sheet2!$E$2:$F$21,MATCH(G40,Sheet2!$F$2:F58,0),1)</f>
+        <f t="array" ref="M40">INDEX(Sheet2!$E$2:$F$21,MATCH(G40,Sheet2!$F$2:F56,0),1)</f>
         <v>.dat</v>
       </c>
       <c r="N40" s="15" t="s">
@@ -4309,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T40" s="16">
         <v>0</v>
@@ -4318,50 +4316,50 @@
         <v>0</v>
       </c>
       <c r="V40" s="15" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="15">
       <c r="A41" s="15" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B41" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>53</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="J41" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K41" s="19">
-        <f t="array" ref="K41">INDEX(Sheet2!$H$2:$I$21,MATCH(G41,Sheet2!$I$2:I44,0),1)</f>
+        <f t="array" ref="K41">INDEX(Sheet2!$H$2:$I$21,MATCH(G41,Sheet2!$I$2:I42,0),1)</f>
         <v>25</v>
       </c>
       <c r="L41" s="20" t="str">
-        <f t="array" ref="L41">INDEX(Sheet2!$B$2:$C$21,MATCH(G41,Sheet2!$C$2:C59,0),1)</f>
+        <f t="array" ref="L41">INDEX(Sheet2!$B$2:$C$21,MATCH(G41,Sheet2!$C$2:C57,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M41" s="21" t="str">
-        <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F59,0),1)</f>
+        <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F57,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N41" s="15" t="s">
@@ -4380,24 +4378,24 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
       </c>
       <c r="U41" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" s="15" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15">
       <c r="A42" s="15" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B42" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" s="16">
         <v>1</v>
@@ -4406,43 +4404,43 @@
         <v>29</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="J42" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K42" s="19">
-        <f t="array" ref="K42">INDEX(Sheet2!$H$2:$I$21,MATCH(G42,Sheet2!$I$2:I45,0),1)</f>
+        <f t="array" ref="K42">INDEX(Sheet2!$H$2:$I$21,MATCH(G42,Sheet2!$I$2:I43,0),1)</f>
         <v>3</v>
       </c>
       <c r="L42" s="20" t="str">
-        <f t="array" ref="L42">INDEX(Sheet2!$B$2:$C$21,MATCH(G42,Sheet2!$C$2:C60,0),1)</f>
+        <f t="array" ref="L42">INDEX(Sheet2!$B$2:$C$21,MATCH(G42,Sheet2!$C$2:C58,0),1)</f>
         <v>b</v>
       </c>
       <c r="M42" s="21" t="str">
-        <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F60,0),1)</f>
+        <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F58,0),1)</f>
         <v>.dat</v>
       </c>
       <c r="N42" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="16">
         <v>1</v>
@@ -4451,62 +4449,62 @@
         <v>1</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
       </c>
       <c r="U42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V42" s="15" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="B43" s="16">
-        <v>22</v>
-      </c>
-      <c r="C43" s="16">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="C43" s="25">
+        <v>18</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>232</v>
+        <v>192</v>
       </c>
       <c r="J43" s="16">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K43" s="19">
-        <f t="array" ref="K43">INDEX(Sheet2!$H$2:$I$21,MATCH(G43,Sheet2!$I$2:I46,0),1)</f>
-        <v>37</v>
+        <f t="array" ref="K43">INDEX(Sheet2!$H$2:$I$21,MATCH(G43,Sheet2!$I$2:I38,0),1)</f>
+        <v>25</v>
       </c>
       <c r="L43" s="20" t="str">
-        <f t="array" ref="L43">INDEX(Sheet2!$B$2:$C$21,MATCH(G43,Sheet2!$C$2:C61,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="L43">INDEX(Sheet2!$B$2:$C$21,MATCH(G43,Sheet2!$C$2:C53,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M43" s="21" t="str">
-        <f t="array" ref="M43">INDEX(Sheet2!$E$2:$F$21,MATCH(G43,Sheet2!$F$2:F61,0),1)</f>
-        <v>.log</v>
-      </c>
-      <c r="N43" s="18" t="s">
+        <f t="array" ref="M43">INDEX(Sheet2!$E$2:$F$21,MATCH(G43,Sheet2!$F$2:F53,0),1)</f>
+        <v>.txt</v>
+      </c>
+      <c r="N43" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O43" s="16">
@@ -4522,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>233</v>
+        <v>28</v>
       </c>
       <c r="T43" s="16">
         <v>0</v>
@@ -4531,60 +4529,59 @@
         <v>1</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="15">
       <c r="A44" s="15" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="B44" s="16">
-        <v>23</v>
-      </c>
-      <c r="C44" s="16">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="C44" s="25">
+        <v>8</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="J44" s="16">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K44" s="19">
-        <f t="array" ref="K44">INDEX(Sheet2!$H$2:$I$21,MATCH(G44,Sheet2!$I$2:I47,0),1)</f>
-        <v>28</v>
-      </c>
-      <c r="L44" s="20" t="str">
-        <f t="array" ref="L44">INDEX(Sheet2!$B$2:$C$21,MATCH(G44,Sheet2!$C$2:C62,0),1)</f>
-        <v>cdr</v>
+        <f t="array" ref="K44">INDEX(Sheet2!$H$2:$I$21,MATCH(G44,Sheet2!$I$2:I39,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L44" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="M44" s="21" t="str">
-        <f t="array" ref="M44">INDEX(Sheet2!$E$2:$F$21,MATCH(G44,Sheet2!$F$2:F62,0),1)</f>
-        <v>.csv</v>
+        <f t="array" ref="M44">INDEX(Sheet2!$E$2:$F$21,MATCH(G44,Sheet2!$F$2:F54,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="O44" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="16">
         <v>1</v>
@@ -4593,60 +4590,60 @@
         <v>1</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="T44" s="16">
         <v>0</v>
       </c>
       <c r="U44" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V44" s="15" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="B45" s="16">
-        <v>23</v>
-      </c>
-      <c r="C45" s="16">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C45" s="25">
+        <v>10</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="J45" s="16">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K45" s="19">
-        <f t="array" ref="K45">INDEX(Sheet2!$H$2:$I$21,MATCH(G45,Sheet2!$I$2:I48,0),1)</f>
-        <v>36</v>
+        <f t="array" ref="K45">INDEX(Sheet2!$H$2:$I$21,MATCH(G45,Sheet2!$I$2:I53,0),1)</f>
+        <v>27</v>
       </c>
       <c r="L45" s="20" t="str">
-        <f t="array" ref="L45">INDEX(Sheet2!$B$2:$C$21,MATCH(G45,Sheet2!$C$2:C63,0),1)</f>
-        <v>CF</v>
+        <f t="array" ref="L45">INDEX(Sheet2!$B$2:$C$21,MATCH(G45,Sheet2!$C$2:C68,0),1)</f>
+        <v>sdr</v>
       </c>
       <c r="M45" s="21" t="str">
-        <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F63,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F68,0),1)</f>
+        <v>.gz</v>
       </c>
       <c r="N45" s="15" t="s">
         <v>27</v>
@@ -4664,69 +4661,69 @@
         <v>1</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>244</v>
+        <v>43</v>
       </c>
       <c r="T45" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="16">
         <v>1</v>
       </c>
       <c r="V45" s="15" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="B46" s="16">
-        <v>24</v>
-      </c>
-      <c r="C46" s="16">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="C46" s="25">
+        <v>9</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="J46" s="16">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K46" s="19">
-        <f t="array" ref="K46">INDEX(Sheet2!$H$2:$I$21,MATCH(G46,Sheet2!$I$2:I49,0),1)</f>
-        <v>27</v>
+        <f t="array" ref="K46">INDEX(Sheet2!$H$2:$I$21,MATCH(G46,Sheet2!$I$2:I54,0),1)</f>
+        <v>17</v>
       </c>
       <c r="L46" s="20" t="str">
-        <f t="array" ref="L46">INDEX(Sheet2!$B$2:$C$21,MATCH(G46,Sheet2!$C$2:C64,0),1)</f>
-        <v>sdr</v>
+        <f t="array" ref="L46">INDEX(Sheet2!$B$2:$C$21,MATCH(G46,Sheet2!$C$2:C69,0),1)</f>
+        <v>ICX</v>
       </c>
       <c r="M46" s="21" t="str">
-        <f t="array" ref="M46">INDEX(Sheet2!$E$2:$F$21,MATCH(G46,Sheet2!$F$2:F64,0),1)</f>
-        <v>.gz</v>
+        <f t="array" ref="M46">INDEX(Sheet2!$E$2:$F$21,MATCH(G46,Sheet2!$F$2:F69,0),1)</f>
+        <v>.DAT</v>
       </c>
       <c r="N46" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O46" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" s="16">
         <v>1</v>
@@ -4735,67 +4732,69 @@
         <v>1</v>
       </c>
       <c r="S46" s="15" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
       <c r="T46" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U46" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="B47" s="16">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C47" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>241</v>
+        <v>53</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>330</v>
+        <v>221</v>
       </c>
       <c r="J47" s="16">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K47" s="19">
-        <v>74</v>
-      </c>
-      <c r="L47" s="20" t="s">
-        <v>328</v>
+        <f t="array" ref="K47">INDEX(Sheet2!$H$2:$I$21,MATCH(G47,Sheet2!$I$2:I44,0),1)</f>
+        <v>25</v>
+      </c>
+      <c r="L47" s="20" t="str">
+        <f t="array" ref="L47">INDEX(Sheet2!$B$2:$C$21,MATCH(G47,Sheet2!$C$2:C59,0),1)</f>
+        <v>esdr</v>
       </c>
       <c r="M47" s="21" t="str">
-        <f t="array" ref="M47">INDEX(Sheet2!$E$2:$F$21,MATCH(G47,Sheet2!$F$2:F65,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M47">INDEX(Sheet2!$E$2:$F$21,MATCH(G47,Sheet2!$F$2:F59,0),1)</f>
+        <v>.txt</v>
       </c>
       <c r="N47" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q47" s="16">
         <v>1</v>
@@ -4804,64 +4803,69 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>331</v>
+        <v>222</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
       </c>
       <c r="U47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15">
       <c r="A48" s="15" t="s">
-        <v>308</v>
+        <v>217</v>
       </c>
       <c r="B48" s="16">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C48" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>309</v>
+        <v>224</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>256</v>
+        <v>46</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>311</v>
+        <v>226</v>
       </c>
       <c r="J48" s="16">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K48" s="19">
-        <v>55</v>
-      </c>
-      <c r="L48" s="20">
-        <v>2</v>
-      </c>
-      <c r="M48" s="21"/>
+        <f t="array" ref="K48">INDEX(Sheet2!$H$2:$I$21,MATCH(G48,Sheet2!$I$2:I45,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L48" s="20" t="str">
+        <f t="array" ref="L48">INDEX(Sheet2!$B$2:$C$21,MATCH(G48,Sheet2!$C$2:C60,0),1)</f>
+        <v>b</v>
+      </c>
+      <c r="M48" s="21" t="str">
+        <f t="array" ref="M48">INDEX(Sheet2!$E$2:$F$21,MATCH(G48,Sheet2!$F$2:F60,0),1)</f>
+        <v>.dat</v>
+      </c>
       <c r="N48" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O48" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P48" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="16">
         <v>1</v>
@@ -4870,68 +4874,69 @@
         <v>1</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>315</v>
+        <v>227</v>
       </c>
       <c r="T48" s="16">
         <v>0</v>
       </c>
       <c r="U48" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="15" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>308</v>
+        <v>217</v>
       </c>
       <c r="B49" s="16">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C49" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>310</v>
+        <v>229</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>312</v>
+        <v>231</v>
       </c>
       <c r="J49" s="16">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K49" s="19">
-        <f t="array" ref="K49">INDEX(Sheet2!$H$2:$I$21,MATCH(G49,Sheet2!$I$2:I52,0),1)</f>
-        <v>3</v>
-      </c>
-      <c r="L49" s="20">
-        <v>2</v>
+        <f t="array" ref="K49">INDEX(Sheet2!$H$2:$I$21,MATCH(G49,Sheet2!$I$2:I46,0),1)</f>
+        <v>37</v>
+      </c>
+      <c r="L49" s="20" t="str">
+        <f t="array" ref="L49">INDEX(Sheet2!$B$2:$C$21,MATCH(G49,Sheet2!$C$2:C61,0),1)</f>
+        <v>cdr</v>
       </c>
       <c r="M49" s="21" t="str">
-        <f t="array" ref="M49">INDEX(Sheet2!$E$2:$F$21,MATCH(G49,Sheet2!$F$2:F67,0),1)</f>
-        <v>.dat</v>
-      </c>
-      <c r="N49" s="15" t="s">
+        <f t="array" ref="M49">INDEX(Sheet2!$E$2:$F$21,MATCH(G49,Sheet2!$F$2:F61,0),1)</f>
+        <v>.log</v>
+      </c>
+      <c r="N49" s="18" t="s">
         <v>27</v>
       </c>
       <c r="O49" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="16">
         <v>1</v>
@@ -4940,69 +4945,64 @@
         <v>1</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>301</v>
+        <v>232</v>
       </c>
       <c r="T49" s="16">
         <v>0</v>
       </c>
       <c r="U49" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="B50" s="16">
-        <v>26</v>
-      </c>
-      <c r="C50" s="25">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="C50" s="16">
+        <v>2</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>263</v>
+        <v>308</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>40</v>
+        <v>255</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
       <c r="J50" s="16">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K50" s="19">
-        <f t="array" ref="K50">INDEX(Sheet2!$H$2:$I$21,MATCH(G50,Sheet2!$I$2:I53,0),1)</f>
-        <v>27</v>
-      </c>
-      <c r="L50" s="20" t="str">
-        <f t="array" ref="L50">INDEX(Sheet2!$B$2:$C$21,MATCH(G50,Sheet2!$C$2:C68,0),1)</f>
-        <v>sdr</v>
-      </c>
-      <c r="M50" s="21" t="str">
-        <f t="array" ref="M50">INDEX(Sheet2!$E$2:$F$21,MATCH(G50,Sheet2!$F$2:F68,0),1)</f>
-        <v>.gz</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="L50" s="20">
+        <v>2</v>
+      </c>
+      <c r="M50" s="21"/>
       <c r="N50" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O50" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="16">
         <v>1</v>
@@ -5011,60 +5011,59 @@
         <v>1</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>43</v>
+        <v>314</v>
       </c>
       <c r="T50" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U50" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="B51" s="16">
-        <v>26</v>
-      </c>
-      <c r="C51" s="25">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="C51" s="16">
+        <v>1</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="J51" s="16">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K51" s="19">
-        <f t="array" ref="K51">INDEX(Sheet2!$H$2:$I$21,MATCH(G51,Sheet2!$I$2:I54,0),1)</f>
-        <v>17</v>
-      </c>
-      <c r="L51" s="20" t="str">
-        <f t="array" ref="L51">INDEX(Sheet2!$B$2:$C$21,MATCH(G51,Sheet2!$C$2:C69,0),1)</f>
-        <v>ICX</v>
+        <f t="array" ref="K51">INDEX(Sheet2!$H$2:$I$21,MATCH(G51,Sheet2!$I$2:I52,0),1)</f>
+        <v>3</v>
+      </c>
+      <c r="L51" s="20">
+        <v>2</v>
       </c>
       <c r="M51" s="21" t="str">
-        <f t="array" ref="M51">INDEX(Sheet2!$E$2:$F$21,MATCH(G51,Sheet2!$F$2:F69,0),1)</f>
-        <v>.DAT</v>
+        <f t="array" ref="M51">INDEX(Sheet2!$E$2:$F$21,MATCH(G51,Sheet2!$F$2:F67,0),1)</f>
+        <v>.dat</v>
       </c>
       <c r="N51" s="15" t="s">
         <v>27</v>
@@ -5082,7 +5081,7 @@
         <v>1</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="T51" s="16">
         <v>0</v>
@@ -5091,12 +5090,12 @@
         <v>0</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B52" s="16">
         <v>27</v>
@@ -5108,19 +5107,19 @@
         <v>4</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>271</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>272</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H52" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="I52" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>274</v>
       </c>
       <c r="J52" s="16">
         <v>27</v>
@@ -5162,12 +5161,12 @@
         <v>1</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15">
       <c r="A53" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B53" s="16">
         <v>27</v>
@@ -5179,19 +5178,19 @@
         <v>29</v>
       </c>
       <c r="E53" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>275</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>276</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H53" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="I53" s="15" t="s">
         <v>277</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>278</v>
       </c>
       <c r="J53" s="16">
         <v>27</v>
@@ -5223,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="S53" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="T53" s="16">
         <v>0</v>
@@ -5232,10 +5231,13 @@
         <v>0</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:V53">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5259,24 +5261,24 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>279</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>280</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5298,14 +5300,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5320,14 +5322,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5342,14 +5344,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -5364,36 +5366,36 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="5">
         <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5408,36 +5410,36 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8">
         <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5452,24 +5454,24 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11">
         <v>37</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1">
@@ -5477,41 +5479,41 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
         <v>39</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
@@ -5619,7 +5621,7 @@
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
       <c r="C25" s="36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>

</xml_diff>

<commit_message>
Newgeneration Configured for Processing
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="339">
   <si>
     <t>operator</t>
   </si>
@@ -745,9 +745,6 @@
     <t>i:\telcobright\vault\resources\cdr\newGenerationTelecom\tdm</t>
   </si>
   <si>
-    <t>Vault.NokiaDhk</t>
-  </si>
-  <si>
     <t>mothertelecom</t>
   </si>
   <si>
@@ -1037,6 +1034,9 @@
   </si>
   <si>
     <t>Vault.TelcobridgeKhulna</t>
+  </si>
+  <si>
+    <t>Vault.Nokia</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1315,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1327,6 +1323,10 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1547,8 +1547,8 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T4" s="16">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>49</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M5" s="21"/>
       <c r="N5" s="15" t="s">
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="T7" s="16">
         <v>0</v>
@@ -2059,73 +2059,73 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="40" customFormat="1" ht="14.25">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:22" s="38" customFormat="1" ht="14.25">
+      <c r="A8" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="39">
         <v>4</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="39">
         <v>2</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="39">
         <v>4</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="39">
         <v>71</v>
       </c>
-      <c r="L8" s="42" t="str">
+      <c r="L8" s="40" t="str">
         <f t="array" ref="L8">INDEX(Sheet2!$B$2:$C$21,MATCH(G8,Sheet2!$C$2:C27,0),1)</f>
         <v>esdr</v>
       </c>
-      <c r="M8" s="43" t="str">
+      <c r="M8" s="41" t="str">
         <f t="array" ref="M8">INDEX(Sheet2!$E$2:$F$21,MATCH(G8,Sheet2!$F$2:F27,0),1)</f>
         <v>.txt</v>
       </c>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="41">
-        <v>0</v>
-      </c>
-      <c r="P8" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="41">
-        <v>1</v>
-      </c>
-      <c r="R8" s="41">
-        <v>1</v>
-      </c>
-      <c r="S8" s="40" t="s">
+      <c r="O8" s="39">
+        <v>0</v>
+      </c>
+      <c r="P8" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="39">
+        <v>1</v>
+      </c>
+      <c r="R8" s="39">
+        <v>1</v>
+      </c>
+      <c r="S8" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="T8" s="41">
-        <v>0</v>
-      </c>
-      <c r="U8" s="41">
-        <v>0</v>
-      </c>
-      <c r="V8" s="40" t="s">
+      <c r="T8" s="39">
+        <v>0</v>
+      </c>
+      <c r="U8" s="39">
+        <v>0</v>
+      </c>
+      <c r="V8" s="38" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T9" s="16">
         <v>1</v>
@@ -2284,16 +2284,16 @@
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="I11" s="35" t="s">
         <v>323</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>324</v>
       </c>
       <c r="J11" s="27">
         <v>12</v>
@@ -2302,7 +2302,7 @@
         <v>68</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M11" s="21" t="str">
         <f t="array" ref="M11">INDEX(Sheet2!$E$2:$F$21,MATCH(G11,Sheet2!$F$2:F42,0),1)</f>
@@ -2324,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="T11" s="27">
         <v>0</v>
@@ -2350,10 +2350,10 @@
         <v>29</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>46</v>
@@ -2362,7 +2362,7 @@
         <v>141</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J12" s="16">
         <v>12</v>
@@ -2371,7 +2371,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M12" s="21" t="str">
         <f t="array" ref="M12">INDEX(Sheet2!$E$2:$F$21,MATCH(G12,Sheet2!$F$2:F43,0),1)</f>
@@ -2393,7 +2393,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T12" s="16">
         <v>0</v>
@@ -2675,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T16" s="16">
         <v>0</v>
@@ -2722,7 +2722,7 @@
         <v>70</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M17" s="21"/>
       <c r="N17" s="15" t="s">
@@ -2764,7 +2764,7 @@
         <v>80</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>81</v>
@@ -2773,7 +2773,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J18" s="16">
         <v>6</v>
@@ -2782,7 +2782,7 @@
         <v>57</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M18" s="21" t="str">
         <f t="array" ref="M18">INDEX(Sheet2!$E$2:$F$21,MATCH(G18,Sheet2!$F$2:F30,0),1)</f>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T18" s="16">
         <v>0</v>
@@ -2830,19 +2830,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>81</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I19" s="35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J19" s="16">
         <v>6</v>
@@ -2851,7 +2851,7 @@
         <v>57</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M19" s="21" t="str">
         <f t="array" ref="M19">INDEX(Sheet2!$E$2:$F$21,MATCH(G19,Sheet2!$F$2:F31,0),1)</f>
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="T19" s="16">
         <v>0</v>
@@ -3134,7 +3134,7 @@
         <v>17</v>
       </c>
       <c r="L23" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M23" s="21" t="str">
         <f t="array" ref="M23">INDEX(Sheet2!$E$2:$F$21,MATCH(G23,Sheet2!$F$2:F35,0),1)</f>
@@ -3557,7 +3557,7 @@
         <v>68</v>
       </c>
       <c r="L29" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M29" s="21" t="str">
         <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F41,0),1)</f>
@@ -3579,7 +3579,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B30" s="16">
         <v>24</v>
@@ -3605,19 +3605,19 @@
         <v>4</v>
       </c>
       <c r="E30" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>244</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I30" s="15" t="s">
         <v>245</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>246</v>
       </c>
       <c r="J30" s="16">
         <v>24</v>
@@ -3650,7 +3650,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T30" s="16">
         <v>1</v>
@@ -3659,12 +3659,12 @@
         <v>1</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B31" s="16">
         <v>24</v>
@@ -3676,19 +3676,19 @@
         <v>29</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>248</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>249</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>238</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J31" s="16">
         <v>24</v>
@@ -3697,7 +3697,7 @@
         <v>74</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M31" s="21" t="str">
         <f t="array" ref="M31">INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F65,0),1)</f>
@@ -3719,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="T31" s="16">
         <v>0</v>
@@ -3728,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
@@ -3834,12 +3834,10 @@
         <v>23</v>
       </c>
       <c r="K33" s="19">
-        <f t="array" ref="K33">INDEX(Sheet2!$H$2:$I$21,MATCH(G33,Sheet2!$I$2:I48,0),1)</f>
-        <v>36</v>
-      </c>
-      <c r="L33" s="20" t="str">
-        <f t="array" ref="L33">INDEX(Sheet2!$B$2:$C$21,MATCH(G33,Sheet2!$C$2:C63,0),1)</f>
-        <v>CF</v>
+        <v>74</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>324</v>
       </c>
       <c r="M33" s="21" t="str">
         <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F63,0),1)</f>
@@ -3849,10 +3847,10 @@
         <v>27</v>
       </c>
       <c r="O33" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="16">
         <v>1</v>
@@ -3861,13 +3859,13 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>241</v>
+        <v>338</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
       </c>
       <c r="U33" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V33" s="15" t="s">
         <v>231</v>
@@ -3980,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M35" s="21" t="str">
         <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F45,0),1)</f>
@@ -4002,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="S35" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T35" s="16">
         <v>0</v>
@@ -4121,7 +4119,7 @@
         <v>3</v>
       </c>
       <c r="L37" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M37" s="21" t="str">
         <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F47,0),1)</f>
@@ -4143,7 +4141,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
@@ -4193,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N38" s="15" t="s">
         <v>27</v>
@@ -4211,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4259,7 +4257,7 @@
         <v>17</v>
       </c>
       <c r="L39" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M39" s="21" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F49,0),1)</f>
@@ -4281,7 +4279,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
@@ -4400,7 +4398,7 @@
         <v>3</v>
       </c>
       <c r="L41" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M41" s="21" t="str">
         <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F56,0),1)</f>
@@ -4422,7 +4420,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
@@ -4564,7 +4562,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T43" s="16">
         <v>0</v>
@@ -4683,7 +4681,7 @@
         <v>3</v>
       </c>
       <c r="L45" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M45" s="21" t="str">
         <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F54,0),1)</f>
@@ -4719,7 +4717,7 @@
     </row>
     <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B46" s="16">
         <v>26</v>
@@ -4731,19 +4729,19 @@
         <v>4</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F46" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H46" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I46" s="15" t="s">
         <v>261</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>262</v>
       </c>
       <c r="J46" s="16">
         <v>26</v>
@@ -4785,12 +4783,12 @@
         <v>1</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B47" s="16">
         <v>26</v>
@@ -4802,19 +4800,19 @@
         <v>29</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F47" s="15" t="s">
         <v>263</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>264</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>101</v>
       </c>
       <c r="H47" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="I47" s="15" t="s">
         <v>265</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>266</v>
       </c>
       <c r="J47" s="16">
         <v>26</v>
@@ -4847,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
@@ -4856,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="15">
@@ -5074,7 +5072,7 @@
     </row>
     <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B51" s="16">
         <v>25</v>
@@ -5086,19 +5084,19 @@
         <v>4</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G51" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="G51" s="17" t="s">
+      <c r="H51" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="H51" s="15" t="s">
-        <v>254</v>
-      </c>
       <c r="I51" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J51" s="16">
         <v>25</v>
@@ -5126,7 +5124,7 @@
         <v>1</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T51" s="16">
         <v>0</v>
@@ -5135,12 +5133,12 @@
         <v>0</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B52" s="16">
         <v>25</v>
@@ -5152,19 +5150,19 @@
         <v>29</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J52" s="16">
         <v>25</v>
@@ -5196,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="S52" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T52" s="16">
         <v>0</v>
@@ -5205,12 +5203,12 @@
         <v>0</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15">
       <c r="A53" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" s="16">
         <v>27</v>
@@ -5222,19 +5220,19 @@
         <v>4</v>
       </c>
       <c r="E53" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>268</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H53" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="I53" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>271</v>
       </c>
       <c r="J53" s="16">
         <v>27</v>
@@ -5276,12 +5274,12 @@
         <v>1</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="15">
       <c r="A54" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B54" s="16">
         <v>27</v>
@@ -5293,19 +5291,19 @@
         <v>29</v>
       </c>
       <c r="E54" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>272</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>273</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H54" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="I54" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="J54" s="16">
         <v>27</v>
@@ -5337,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="S54" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T54" s="16">
         <v>0</v>
@@ -5346,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="V54" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5376,24 +5374,24 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>276</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>277</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5415,14 +5413,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5437,14 +5435,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5459,14 +5457,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -5481,14 +5479,14 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>101</v>
@@ -5503,14 +5501,14 @@
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5525,14 +5523,14 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>238</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>238</v>
@@ -5547,14 +5545,14 @@
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5569,14 +5567,14 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>81</v>
@@ -5594,31 +5592,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>164</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>164</v>
@@ -5735,27 +5733,27 @@
     <row r="23" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C25" s="38" t="s">
-        <v>293</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
+      <c r="C25" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
     </row>
     <row r="26" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
     </row>
     <row r="27" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
     </row>
     <row r="28" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="29" spans="2:9" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
purple,softex,imamnetwork ne settings and directory upadated
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/_helper/casOperatorInfo.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9276"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="NE automation data" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -646,9 +649,6 @@
     <t>i:\telcobright\vault\resources\cdr\softex\ip</t>
   </si>
   <si>
-    <t>softex_10.255.200.52_CATALEYA</t>
-  </si>
-  <si>
     <t>10.154.150.52</t>
   </si>
   <si>
@@ -1034,6 +1034,9 @@
   </si>
   <si>
     <t>vault.Reve</t>
+  </si>
+  <si>
+    <t>Vault.Zte</t>
   </si>
 </sst>
 </file>
@@ -1406,6 +1409,224 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="NE automation data"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>b</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>HUWAEI</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>.dat</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>HUWAEI</v>
+          </cell>
+          <cell r="H2">
+            <v>3</v>
+          </cell>
+          <cell r="I2" t="str">
+            <v>HUWAEI</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>VCDR</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>GENBAND</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>.gz</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>GENBAND</v>
+          </cell>
+          <cell r="H3">
+            <v>31</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>GENBAND</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>esdr</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>CATALEYA</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>.txt</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>CATALEYA</v>
+          </cell>
+          <cell r="H4">
+            <v>25</v>
+          </cell>
+          <cell r="I4" t="str">
+            <v>CATALEYA</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>ICX</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>ZTE</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>.DAT</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>ZTE</v>
+          </cell>
+          <cell r="H5">
+            <v>17</v>
+          </cell>
+          <cell r="I5" t="str">
+            <v>ZTE</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>cdr</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>REVE</v>
+          </cell>
+          <cell r="E6" t="str">
+            <v>.csv</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>REVE</v>
+          </cell>
+          <cell r="H6">
+            <v>28</v>
+          </cell>
+          <cell r="I6" t="str">
+            <v>REVE</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>CF</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>NOKIA</v>
+          </cell>
+          <cell r="E7" t="str">
+            <v>.DAT</v>
+          </cell>
+          <cell r="F7" t="str">
+            <v>NOKIA</v>
+          </cell>
+          <cell r="H7">
+            <v>36</v>
+          </cell>
+          <cell r="I7" t="str">
+            <v>NOKIA</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>sdr</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>DIALOGIC</v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>.gz</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>DIALOGIC</v>
+          </cell>
+          <cell r="H8">
+            <v>27</v>
+          </cell>
+          <cell r="I8" t="str">
+            <v>DIALOGIC</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>cdr</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>TELCOBRIDGE</v>
+          </cell>
+          <cell r="E9" t="str">
+            <v>.log</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>TELCOBRIDGE</v>
+          </cell>
+          <cell r="H9">
+            <v>37</v>
+          </cell>
+          <cell r="I9" t="str">
+            <v>TELCOBRIDGE</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>2</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>WTL</v>
+          </cell>
+          <cell r="F10" t="str">
+            <v>WTL</v>
+          </cell>
+          <cell r="H10">
+            <v>38</v>
+          </cell>
+          <cell r="I10" t="str">
+            <v>WTL</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>CDR</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>GNEW</v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>.csv</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>GNEW</v>
+          </cell>
+          <cell r="H11">
+            <v>39</v>
+          </cell>
+          <cell r="I11" t="str">
+            <v>GNEW</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25" t="str">
+            <v>PLEASE DO NOT MODIFY ANYTHING IN THIS SHEET</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1607,32 +1828,32 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickTop="1" thickBot="1">
+    <row r="1" spans="1:22" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1700,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" thickTop="1">
+    <row r="2" spans="1:22" ht="15.75" thickTop="1">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.4">
+    <row r="3" spans="1:22" ht="15">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -1829,7 +2050,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -1841,7 +2062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="14.4">
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="15" t="s">
         <v>49</v>
       </c>
@@ -1899,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T4" s="16">
         <v>0</v>
@@ -1911,7 +2132,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="14.4">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="15" t="s">
         <v>49</v>
       </c>
@@ -1946,7 +2167,7 @@
         <v>49</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M5" s="21"/>
       <c r="N5" s="15" t="s">
@@ -1977,7 +2198,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14.4">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="15" t="s">
         <v>37</v>
       </c>
@@ -2048,7 +2269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.4">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="15" t="s">
         <v>37</v>
       </c>
@@ -2107,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T7" s="16">
         <v>0</v>
@@ -2119,7 +2340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="38" customFormat="1" ht="13.8">
+    <row r="8" spans="1:22" s="38" customFormat="1" ht="14.25">
       <c r="A8" s="38" t="s">
         <v>60</v>
       </c>
@@ -2189,7 +2410,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.4">
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="15" t="s">
         <v>60</v>
       </c>
@@ -2248,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="S9" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T9" s="16">
         <v>1</v>
@@ -2260,7 +2481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.4">
+    <row r="10" spans="1:22" ht="15">
       <c r="A10" s="26" t="s">
         <v>133</v>
       </c>
@@ -2329,7 +2550,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.4">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="26" t="s">
         <v>133</v>
       </c>
@@ -2344,16 +2565,16 @@
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="I11" s="35" t="s">
         <v>317</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>318</v>
       </c>
       <c r="J11" s="27">
         <v>12</v>
@@ -2362,7 +2583,7 @@
         <v>68</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M11" s="21" t="str">
         <f t="array" ref="M11">INDEX(Sheet2!$E$2:$F$21,MATCH(G11,Sheet2!$F$2:F42,0),1)</f>
@@ -2384,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T11" s="27">
         <v>0</v>
@@ -2396,7 +2617,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="14.4">
+    <row r="12" spans="1:22" ht="15">
       <c r="A12" s="15" t="s">
         <v>133</v>
       </c>
@@ -2410,10 +2631,10 @@
         <v>29</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>46</v>
@@ -2422,7 +2643,7 @@
         <v>139</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J12" s="16">
         <v>12</v>
@@ -2431,7 +2652,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M12" s="21" t="str">
         <f t="array" ref="M12">INDEX(Sheet2!$E$2:$F$21,MATCH(G12,Sheet2!$F$2:F43,0),1)</f>
@@ -2453,7 +2674,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T12" s="16">
         <v>0</v>
@@ -2465,7 +2686,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="48" customFormat="1" ht="14.4">
+    <row r="13" spans="1:22" s="48" customFormat="1" ht="15">
       <c r="A13" s="42" t="s">
         <v>169</v>
       </c>
@@ -2523,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T13" s="43">
         <v>0</v>
@@ -2535,7 +2756,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="14.4">
+    <row r="14" spans="1:22" ht="15">
       <c r="A14" s="15" t="s">
         <v>169</v>
       </c>
@@ -2606,7 +2827,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="14.4">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="15" t="s">
         <v>169</v>
       </c>
@@ -2677,7 +2898,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.4">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="15" t="s">
         <v>70</v>
       </c>
@@ -2735,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T16" s="16">
         <v>0</v>
@@ -2747,7 +2968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="14.4">
+    <row r="17" spans="1:22" ht="15">
       <c r="A17" s="15" t="s">
         <v>70</v>
       </c>
@@ -2782,7 +3003,7 @@
         <v>70</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M17" s="21"/>
       <c r="N17" s="15" t="s">
@@ -2813,7 +3034,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="36" customFormat="1" ht="14.4">
+    <row r="18" spans="1:22" s="36" customFormat="1" ht="15">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2824,7 +3045,7 @@
         <v>79</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>80</v>
@@ -2833,7 +3054,7 @@
         <v>81</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J18" s="16">
         <v>6</v>
@@ -2842,7 +3063,7 @@
         <v>57</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M18" s="21" t="str">
         <f t="array" ref="M18">INDEX(Sheet2!$E$2:$F$21,MATCH(G18,Sheet2!$F$2:F30,0),1)</f>
@@ -2864,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="T18" s="16">
         <v>0</v>
@@ -2876,7 +3097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="14.4">
+    <row r="19" spans="1:22" ht="15">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -2890,19 +3111,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>80</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I19" s="35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J19" s="16">
         <v>6</v>
@@ -2911,7 +3132,7 @@
         <v>57</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M19" s="21" t="str">
         <f t="array" ref="M19">INDEX(Sheet2!$E$2:$F$21,MATCH(G19,Sheet2!$F$2:F31,0),1)</f>
@@ -2933,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="T19" s="16">
         <v>0</v>
@@ -2945,7 +3166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="14.4">
+    <row r="20" spans="1:22" ht="15">
       <c r="A20" s="15" t="s">
         <v>82</v>
       </c>
@@ -3016,7 +3237,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="14.4">
+    <row r="21" spans="1:22" ht="15">
       <c r="A21" s="15" t="s">
         <v>82</v>
       </c>
@@ -3087,7 +3308,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="14.4">
+    <row r="22" spans="1:22" ht="15">
       <c r="A22" s="15" t="s">
         <v>93</v>
       </c>
@@ -3119,25 +3340,25 @@
         <v>8</v>
       </c>
       <c r="K22" s="19">
-        <f t="array" ref="K22">INDEX(Sheet2!$H$2:$I$21,MATCH(G22,Sheet2!$I$2:I19,0),1)</f>
+        <f t="array" ref="K22">INDEX([1]Sheet2!$H$2:$I$21,MATCH(G22,[1]Sheet2!$I$2:I19,0),1)</f>
         <v>25</v>
       </c>
       <c r="L22" s="20" t="str">
-        <f t="array" ref="L22">INDEX(Sheet2!$B$2:$C$21,MATCH(G22,Sheet2!$C$2:C34,0),1)</f>
+        <f t="array" ref="L22">INDEX([1]Sheet2!$B$2:$C$21,MATCH(G22,[1]Sheet2!$C$2:C34,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M22" s="21" t="str">
-        <f t="array" ref="M22">INDEX(Sheet2!$E$2:$F$21,MATCH(G22,Sheet2!$F$2:F34,0),1)</f>
+        <f t="array" ref="M22">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G22,[1]Sheet2!$F$2:F34,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N22" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="16">
         <v>1</v>
@@ -3146,19 +3367,19 @@
         <v>1</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>108</v>
+        <v>322</v>
       </c>
       <c r="T22" s="16">
         <v>0</v>
       </c>
       <c r="U22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="14.4">
+    <row r="23" spans="1:22" ht="15">
       <c r="A23" s="15" t="s">
         <v>93</v>
       </c>
@@ -3190,14 +3411,14 @@
         <v>8</v>
       </c>
       <c r="K23" s="19">
-        <f t="array" ref="K23">INDEX(Sheet2!$H$2:$I$21,MATCH(G23,Sheet2!$I$2:I20,0),1)</f>
+        <f t="array" ref="K23">INDEX([1]Sheet2!$H$2:$I$21,MATCH(G23,[1]Sheet2!$I$2:I20,0),1)</f>
         <v>17</v>
       </c>
       <c r="L23" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M23" s="21" t="str">
-        <f t="array" ref="M23">INDEX(Sheet2!$E$2:$F$21,MATCH(G23,Sheet2!$F$2:F35,0),1)</f>
+        <f t="array" ref="M23">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G23,[1]Sheet2!$F$2:F35,0),1)</f>
         <v>.DAT</v>
       </c>
       <c r="N23" s="15" t="s">
@@ -3216,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>113</v>
+        <v>337</v>
       </c>
       <c r="T23" s="16">
         <v>0</v>
@@ -3228,7 +3449,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="32" customFormat="1" ht="14.4">
+    <row r="24" spans="1:22" s="32" customFormat="1" ht="15">
       <c r="A24" s="15" t="s">
         <v>103</v>
       </c>
@@ -3298,7 +3519,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="32" customFormat="1" ht="14.4">
+    <row r="25" spans="1:22" s="32" customFormat="1" ht="15">
       <c r="A25" s="15" t="s">
         <v>103</v>
       </c>
@@ -3369,7 +3590,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="14.4">
+    <row r="26" spans="1:22" ht="15">
       <c r="A26" s="15" t="s">
         <v>114</v>
       </c>
@@ -3440,7 +3661,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="14.4">
+    <row r="27" spans="1:22" ht="15">
       <c r="A27" s="15" t="s">
         <v>114</v>
       </c>
@@ -3511,7 +3732,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:22" s="49" customFormat="1" ht="13.8">
+    <row r="28" spans="1:22" s="49" customFormat="1" ht="14.25">
       <c r="A28" s="49" t="s">
         <v>124</v>
       </c>
@@ -3569,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="S28" s="49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T28" s="50">
         <v>0</v>
@@ -3581,7 +3802,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="14.4">
+    <row r="29" spans="1:22" ht="15">
       <c r="A29" s="15" t="s">
         <v>124</v>
       </c>
@@ -3616,7 +3837,7 @@
         <v>68</v>
       </c>
       <c r="L29" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M29" s="21" t="str">
         <f t="array" ref="M29">INDEX(Sheet2!$E$2:$F$21,MATCH(G29,Sheet2!$F$2:F41,0),1)</f>
@@ -3638,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T29" s="16">
         <v>0</v>
@@ -3650,9 +3871,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="14.4">
+    <row r="30" spans="1:22" ht="15">
       <c r="A30" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B30" s="16">
         <v>24</v>
@@ -3664,19 +3885,19 @@
         <v>4</v>
       </c>
       <c r="E30" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>240</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="I30" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="J30" s="16">
         <v>24</v>
@@ -3709,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="T30" s="16">
         <v>1</v>
@@ -3718,12 +3939,12 @@
         <v>1</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="14.4">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="15">
       <c r="A31" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B31" s="16">
         <v>24</v>
@@ -3735,19 +3956,19 @@
         <v>29</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="G31" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="H31" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>246</v>
-      </c>
       <c r="I31" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J31" s="16">
         <v>24</v>
@@ -3756,7 +3977,7 @@
         <v>74</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M31" s="21" t="str">
         <f t="array" ref="M31">INDEX(Sheet2!$E$2:$F$21,MATCH(G31,Sheet2!$F$2:F65,0),1)</f>
@@ -3778,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T31" s="16">
         <v>0</v>
@@ -3787,12 +4008,12 @@
         <v>0</v>
       </c>
       <c r="V31" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" s="49" customFormat="1" ht="13.8">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="49" customFormat="1" ht="14.25">
       <c r="A32" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B32" s="50">
         <v>23</v>
@@ -3804,19 +4025,19 @@
         <v>4</v>
       </c>
       <c r="E32" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" s="49" t="s">
         <v>229</v>
-      </c>
-      <c r="F32" s="49" t="s">
-        <v>230</v>
       </c>
       <c r="G32" s="49" t="s">
         <v>24</v>
       </c>
       <c r="H32" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="I32" s="49" t="s">
         <v>231</v>
-      </c>
-      <c r="I32" s="49" t="s">
-        <v>232</v>
       </c>
       <c r="J32" s="50">
         <v>23</v>
@@ -3848,7 +4069,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="49" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T32" s="50">
         <v>0</v>
@@ -3857,12 +4078,12 @@
         <v>0</v>
       </c>
       <c r="V32" s="49" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="14.4">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="15">
       <c r="A33" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B33" s="16">
         <v>23</v>
@@ -3874,19 +4095,19 @@
         <v>29</v>
       </c>
       <c r="E33" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="G33" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="H33" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="I33" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>237</v>
       </c>
       <c r="J33" s="16">
         <v>23</v>
@@ -3895,7 +4116,7 @@
         <v>74</v>
       </c>
       <c r="L33" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M33" s="21" t="str">
         <f t="array" ref="M33">INDEX(Sheet2!$E$2:$F$21,MATCH(G33,Sheet2!$F$2:F63,0),1)</f>
@@ -3917,7 +4138,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="T33" s="16">
         <v>0</v>
@@ -3926,10 +4147,10 @@
         <v>0</v>
       </c>
       <c r="V33" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="14.4">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="15">
       <c r="A34" s="15" t="s">
         <v>140</v>
       </c>
@@ -4000,7 +4221,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="14.4">
+    <row r="35" spans="1:22" ht="15">
       <c r="A35" s="15" t="s">
         <v>140</v>
       </c>
@@ -4036,7 +4257,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M35" s="21" t="str">
         <f t="array" ref="M35">INDEX(Sheet2!$E$2:$F$21,MATCH(G35,Sheet2!$F$2:F45,0),1)</f>
@@ -4058,7 +4279,7 @@
         <v>1</v>
       </c>
       <c r="S35" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T35" s="16">
         <v>0</v>
@@ -4070,7 +4291,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="14.4">
+    <row r="36" spans="1:22" ht="15">
       <c r="A36" s="15" t="s">
         <v>150</v>
       </c>
@@ -4102,25 +4323,24 @@
         <v>16</v>
       </c>
       <c r="K36" s="19">
-        <f t="array" ref="K36">INDEX(Sheet2!$H$2:$I$21,MATCH(G36,Sheet2!$I$2:I31,0),1)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L36" s="20" t="str">
-        <f t="array" ref="L36">INDEX(Sheet2!$B$2:$C$21,MATCH(G36,Sheet2!$C$2:C46,0),1)</f>
+        <f t="array" ref="L36">INDEX([1]Sheet2!$B$2:$C$21,MATCH(G36,[1]Sheet2!$C$2:C46,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M36" s="21" t="str">
-        <f t="array" ref="M36">INDEX(Sheet2!$E$2:$F$21,MATCH(G36,Sheet2!$F$2:F46,0),1)</f>
+        <f t="array" ref="M36">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G36,[1]Sheet2!$F$2:F46,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N36" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="16">
         <v>1</v>
@@ -4129,19 +4349,19 @@
         <v>1</v>
       </c>
       <c r="S36" s="15" t="s">
-        <v>65</v>
+        <v>333</v>
       </c>
       <c r="T36" s="16">
         <v>0</v>
       </c>
       <c r="U36" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V36" s="15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="14.4">
+    <row r="37" spans="1:22" ht="15">
       <c r="A37" s="15" t="s">
         <v>150</v>
       </c>
@@ -4173,14 +4393,14 @@
         <v>16</v>
       </c>
       <c r="K37" s="19">
-        <f t="array" ref="K37">INDEX(Sheet2!$H$2:$I$21,MATCH(G37,Sheet2!$I$2:I32,0),1)</f>
+        <f t="array" ref="K37">INDEX([1]Sheet2!$H$2:$I$21,MATCH(G37,[1]Sheet2!$I$2:I32,0),1)</f>
         <v>3</v>
       </c>
       <c r="L37" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M37" s="21" t="str">
-        <f t="array" ref="M37">INDEX(Sheet2!$E$2:$F$21,MATCH(G37,Sheet2!$F$2:F47,0),1)</f>
+        <f t="array" ref="M37">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G37,[1]Sheet2!$F$2:F47,0),1)</f>
         <v>.dat</v>
       </c>
       <c r="N37" s="15" t="s">
@@ -4199,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T37" s="16">
         <v>0</v>
@@ -4211,7 +4431,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="14.4">
+    <row r="38" spans="1:22" ht="15">
       <c r="A38" s="15" t="s">
         <v>159</v>
       </c>
@@ -4249,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N38" s="15" t="s">
         <v>27</v>
@@ -4267,7 +4487,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T38" s="16">
         <v>0</v>
@@ -4279,7 +4499,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="14.4">
+    <row r="39" spans="1:22" ht="15">
       <c r="A39" s="15" t="s">
         <v>159</v>
       </c>
@@ -4315,7 +4535,7 @@
         <v>17</v>
       </c>
       <c r="L39" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M39" s="21" t="str">
         <f>INDEX(Sheet2!$E$2:$F$21,MATCH(G39,Sheet2!$F$2:F49,0),1)</f>
@@ -4337,7 +4557,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T39" s="16">
         <v>0</v>
@@ -4349,7 +4569,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="14.4">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40" s="15" t="s">
         <v>193</v>
       </c>
@@ -4420,7 +4640,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="14.4">
+    <row r="41" spans="1:22" ht="15">
       <c r="A41" s="15" t="s">
         <v>193</v>
       </c>
@@ -4456,7 +4676,7 @@
         <v>3</v>
       </c>
       <c r="L41" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M41" s="21" t="str">
         <f t="array" ref="M41">INDEX(Sheet2!$E$2:$F$21,MATCH(G41,Sheet2!$F$2:F56,0),1)</f>
@@ -4478,7 +4698,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T41" s="16">
         <v>0</v>
@@ -4490,7 +4710,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="14.4">
+    <row r="42" spans="1:22" ht="15">
       <c r="A42" s="15" t="s">
         <v>203</v>
       </c>
@@ -4522,25 +4742,24 @@
         <v>21</v>
       </c>
       <c r="K42" s="19">
-        <f t="array" ref="K42">INDEX(Sheet2!$H$2:$I$21,MATCH(G42,Sheet2!$I$2:I42,0),1)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L42" s="20" t="str">
-        <f t="array" ref="L42">INDEX(Sheet2!$B$2:$C$21,MATCH(G42,Sheet2!$C$2:C57,0),1)</f>
+        <f t="array" ref="L42">INDEX([1]Sheet2!$B$2:$C$21,MATCH(G42,[1]Sheet2!$C$2:C57,0),1)</f>
         <v>esdr</v>
       </c>
       <c r="M42" s="21" t="str">
-        <f t="array" ref="M42">INDEX(Sheet2!$E$2:$F$21,MATCH(G42,Sheet2!$F$2:F57,0),1)</f>
+        <f t="array" ref="M42">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G42,[1]Sheet2!$F$2:F57,0),1)</f>
         <v>.txt</v>
       </c>
       <c r="N42" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="16">
         <v>1</v>
@@ -4549,7 +4768,7 @@
         <v>1</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>208</v>
+        <v>323</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
@@ -4561,7 +4780,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="14.4">
+    <row r="43" spans="1:22" ht="15">
       <c r="A43" s="15" t="s">
         <v>203</v>
       </c>
@@ -4575,33 +4794,33 @@
         <v>29</v>
       </c>
       <c r="E43" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="15" t="s">
         <v>209</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>210</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H43" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="I43" s="15" t="s">
         <v>211</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>212</v>
       </c>
       <c r="J43" s="16">
         <v>21</v>
       </c>
       <c r="K43" s="19">
-        <f t="array" ref="K43">INDEX(Sheet2!$H$2:$I$21,MATCH(G43,Sheet2!$I$2:I43,0),1)</f>
+        <f t="array" ref="K43">INDEX([1]Sheet2!$H$2:$I$21,MATCH(G43,[1]Sheet2!$I$2:I43,0),1)</f>
         <v>3</v>
       </c>
       <c r="L43" s="20" t="str">
-        <f t="array" ref="L43">INDEX(Sheet2!$B$2:$C$21,MATCH(G43,Sheet2!$C$2:C58,0),1)</f>
+        <f t="array" ref="L43">INDEX([1]Sheet2!$B$2:$C$21,MATCH(G43,[1]Sheet2!$C$2:C58,0),1)</f>
         <v>b</v>
       </c>
       <c r="M43" s="21" t="str">
-        <f t="array" ref="M43">INDEX(Sheet2!$E$2:$F$21,MATCH(G43,Sheet2!$F$2:F58,0),1)</f>
+        <f t="array" ref="M43">INDEX([1]Sheet2!$E$2:$F$21,MATCH(G43,[1]Sheet2!$F$2:F58,0),1)</f>
         <v>.dat</v>
       </c>
       <c r="N43" s="15" t="s">
@@ -4620,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T43" s="16">
         <v>0</v>
@@ -4632,7 +4851,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="14.4">
+    <row r="44" spans="1:22" ht="15">
       <c r="A44" s="15" t="s">
         <v>184</v>
       </c>
@@ -4703,7 +4922,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="14.4">
+    <row r="45" spans="1:22" ht="15">
       <c r="A45" s="15" t="s">
         <v>184</v>
       </c>
@@ -4739,7 +4958,7 @@
         <v>3</v>
       </c>
       <c r="L45" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M45" s="21" t="str">
         <f t="array" ref="M45">INDEX(Sheet2!$E$2:$F$21,MATCH(G45,Sheet2!$F$2:F54,0),1)</f>
@@ -4773,9 +4992,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="14.4">
+    <row r="46" spans="1:22" ht="15">
       <c r="A46" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B46" s="16">
         <v>26</v>
@@ -4787,19 +5006,19 @@
         <v>4</v>
       </c>
       <c r="E46" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="F46" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>256</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H46" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="I46" s="15" t="s">
         <v>257</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>258</v>
       </c>
       <c r="J46" s="16">
         <v>26</v>
@@ -4841,12 +5060,12 @@
         <v>1</v>
       </c>
       <c r="V46" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" ht="14.4">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="15">
       <c r="A47" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B47" s="16">
         <v>26</v>
@@ -4858,19 +5077,19 @@
         <v>29</v>
       </c>
       <c r="E47" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F47" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>100</v>
       </c>
       <c r="H47" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I47" s="15" t="s">
         <v>261</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>262</v>
       </c>
       <c r="J47" s="16">
         <v>26</v>
@@ -4903,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T47" s="16">
         <v>0</v>
@@ -4912,12 +5131,12 @@
         <v>0</v>
       </c>
       <c r="V47" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" s="38" customFormat="1" ht="13.8">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" s="38" customFormat="1" ht="14.25">
       <c r="A48" s="38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48" s="39">
         <v>22</v>
@@ -4929,19 +5148,19 @@
         <v>4</v>
       </c>
       <c r="E48" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" s="38" t="s">
         <v>214</v>
-      </c>
-      <c r="F48" s="38" t="s">
-        <v>215</v>
       </c>
       <c r="G48" s="38" t="s">
         <v>52</v>
       </c>
       <c r="H48" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="I48" s="38" t="s">
         <v>216</v>
-      </c>
-      <c r="I48" s="38" t="s">
-        <v>217</v>
       </c>
       <c r="J48" s="39">
         <v>22</v>
@@ -4973,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="S48" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T48" s="39">
         <v>0</v>
@@ -4982,12 +5201,12 @@
         <v>0</v>
       </c>
       <c r="V48" s="38" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" ht="14.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="15">
       <c r="A49" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" s="16">
         <v>22</v>
@@ -4999,19 +5218,19 @@
         <v>29</v>
       </c>
       <c r="E49" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" s="15" t="s">
         <v>218</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>219</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H49" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="I49" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>221</v>
       </c>
       <c r="J49" s="16">
         <v>22</v>
@@ -5044,7 +5263,7 @@
         <v>1</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T49" s="16">
         <v>0</v>
@@ -5053,12 +5272,12 @@
         <v>1</v>
       </c>
       <c r="V49" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" ht="14.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="15">
       <c r="A50" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" s="16">
         <v>22</v>
@@ -5070,19 +5289,19 @@
         <v>29</v>
       </c>
       <c r="E50" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>80</v>
       </c>
       <c r="H50" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="I50" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>226</v>
       </c>
       <c r="J50" s="16">
         <v>22</v>
@@ -5115,7 +5334,7 @@
         <v>1</v>
       </c>
       <c r="S50" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T50" s="16">
         <v>0</v>
@@ -5124,12 +5343,12 @@
         <v>1</v>
       </c>
       <c r="V50" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" ht="14.4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="15">
       <c r="A51" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B51" s="16">
         <v>25</v>
@@ -5141,19 +5360,19 @@
         <v>4</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="G51" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="G51" s="17" t="s">
+      <c r="H51" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="H51" s="15" t="s">
-        <v>250</v>
-      </c>
       <c r="I51" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J51" s="16">
         <v>25</v>
@@ -5181,7 +5400,7 @@
         <v>1</v>
       </c>
       <c r="S51" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="T51" s="16">
         <v>0</v>
@@ -5190,12 +5409,12 @@
         <v>0</v>
       </c>
       <c r="V51" s="15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" ht="14.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="15">
       <c r="A52" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B52" s="16">
         <v>25</v>
@@ -5207,19 +5426,19 @@
         <v>29</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J52" s="16">
         <v>25</v>
@@ -5251,7 +5470,7 @@
         <v>1</v>
       </c>
       <c r="S52" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T52" s="16">
         <v>0</v>
@@ -5260,12 +5479,12 @@
         <v>0</v>
       </c>
       <c r="V52" s="15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" ht="14.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="15">
       <c r="A53" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B53" s="16">
         <v>27</v>
@@ -5277,19 +5496,19 @@
         <v>4</v>
       </c>
       <c r="E53" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="15" t="s">
         <v>264</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>265</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J53" s="16">
         <v>27</v>
@@ -5321,7 +5540,7 @@
         <v>1</v>
       </c>
       <c r="S53" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T53" s="16">
         <v>0</v>
@@ -5330,12 +5549,12 @@
         <v>0</v>
       </c>
       <c r="V53" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" ht="14.4">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="15">
       <c r="A54" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B54" s="16">
         <v>27</v>
@@ -5347,19 +5566,19 @@
         <v>29</v>
       </c>
       <c r="E54" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>268</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J54" s="16">
         <v>27</v>
@@ -5391,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="S54" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T54" s="16">
         <v>0</v>
@@ -5400,7 +5619,7 @@
         <v>0</v>
       </c>
       <c r="V54" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5420,34 +5639,34 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>270</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>271</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5469,14 +5688,14 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>46</v>
@@ -5491,14 +5710,14 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>32</v>
@@ -5513,14 +5732,14 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>52</v>
@@ -5535,14 +5754,14 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>100</v>
@@ -5557,14 +5776,14 @@
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -5579,36 +5798,36 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1">
       <c r="B7" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8">
         <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
@@ -5623,14 +5842,14 @@
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>80</v>
@@ -5648,31 +5867,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="14"/>
       <c r="F10" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>38</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>162</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>162</v>
@@ -5790,7 +6009,7 @@
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
       <c r="C25" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>

</xml_diff>